<commit_message>
updated BodyPartDefs.xlsx with data
</commit_message>
<xml_diff>
--- a/UnityProject/LD35/Assets/StaticDefinitions/BodyPartDefs.xlsx
+++ b/UnityProject/LD35/Assets/StaticDefinitions/BodyPartDefs.xlsx
@@ -1,23 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LD35\trunk\UnityProject\LD35\Assets\StaticDefinitions\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="22035" windowHeight="9285"/>
+    <workbookView xWindow="120" yWindow="1320" windowWidth="22035" windowHeight="9285" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="HeadPartDefs" sheetId="1" r:id="rId1"/>
+    <sheet name="HeadPartDefs" sheetId="5" r:id="rId1"/>
     <sheet name="ThoraxPartDefs" sheetId="2" r:id="rId2"/>
     <sheet name="AbdomenPartDefs" sheetId="3" r:id="rId3"/>
     <sheet name="LegPartDefs" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="9">
   <si>
     <t>ID</t>
   </si>
@@ -40,22 +46,10 @@
     <t>jumpForce</t>
   </si>
   <si>
-    <t>assetUpperName</t>
-  </si>
-  <si>
-    <t>assetLowerName</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
-    <t>Head</t>
-  </si>
-  <si>
-    <t>Large damage pew pew</t>
-  </si>
-  <si>
-    <t>beetle1-head</t>
+    <t>assetPrefix</t>
   </si>
 </sst>
 </file>
@@ -112,14 +106,220 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="10">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TabHeadParts" displayName="TabHeadParts" ref="A1:H5" totalsRowShown="0" headerRowDxfId="9">
+  <autoFilter ref="A1:H5"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="ID"/>
+    <tableColumn id="2" name="name">
+      <calculatedColumnFormula>CONCATENATE("Beetle Head ",A2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" name="description">
+      <calculatedColumnFormula>CONCATENATE("A ", B2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="assetName">
+      <calculatedColumnFormula>CONCATENATE("beetle",A2,"-head")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="health"/>
+    <tableColumn id="6" name="damage"/>
+    <tableColumn id="7" name="turnSpeed"/>
+    <tableColumn id="8" name="jumpForce"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TabThoraxParts" displayName="TabThoraxParts" ref="A1:H5" totalsRowShown="0" headerRowDxfId="8">
+  <autoFilter ref="A1:H5"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="ID"/>
+    <tableColumn id="2" name="name" dataDxfId="7">
+      <calculatedColumnFormula>CONCATENATE("Beetle Thorax ",A2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" name="description">
+      <calculatedColumnFormula>CONCATENATE("A ", B2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="assetName" dataDxfId="6">
+      <calculatedColumnFormula>CONCATENATE("beetle",A2,"-thorax")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="health"/>
+    <tableColumn id="6" name="damage"/>
+    <tableColumn id="7" name="turnSpeed"/>
+    <tableColumn id="8" name="jumpForce"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="TabAbdomenParts" displayName="TabAbdomenParts" ref="A1:H5" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:H5"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="ID"/>
+    <tableColumn id="2" name="name" dataDxfId="4">
+      <calculatedColumnFormula>CONCATENATE("Beetle Abdomen ",A2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" name="description">
+      <calculatedColumnFormula>CONCATENATE("A ", B2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="assetName" dataDxfId="3">
+      <calculatedColumnFormula>CONCATENATE("beetle",A2,"-abdomen")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="health"/>
+    <tableColumn id="6" name="damage"/>
+    <tableColumn id="7" name="turnSpeed"/>
+    <tableColumn id="8" name="jumpForce"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="TabLegParts" displayName="TabLegParts" ref="A1:H5" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:H5"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="ID"/>
+    <tableColumn id="2" name="name" dataDxfId="0">
+      <calculatedColumnFormula>CONCATENATE("Beetle Leg ",A2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" name="description">
+      <calculatedColumnFormula>CONCATENATE("A ", B2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="assetPrefix" dataDxfId="1">
+      <calculatedColumnFormula>CONCATENATE("beetle",A2,)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="health"/>
+    <tableColumn id="6" name="damage"/>
+    <tableColumn id="7" name="turnSpeed"/>
+    <tableColumn id="8" name="jumpForce"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -165,7 +365,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -200,7 +400,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -408,21 +608,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1"/>
-    <col min="6" max="7" width="15.28515625" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="5" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
     <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -436,7 +638,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -458,23 +660,26 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
+      <c r="B2" t="str">
+        <f>CONCATENATE("Beetle Head ",A2)</f>
+        <v>Beetle Head 1</v>
+      </c>
+      <c r="C2" t="str">
+        <f>CONCATENATE("A ", B2)</f>
+        <v>A Beetle Head 1</v>
+      </c>
+      <c r="D2" t="str">
+        <f>CONCATENATE("beetle",A2,"-head")</f>
+        <v>beetle1-head</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -484,47 +689,116 @@
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B5" si="0">CONCATENATE("Beetle Head ",A3)</f>
+        <v>Beetle Head 2</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C5" si="1">CONCATENATE("A ", B3)</f>
+        <v>A Beetle Head 2</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D5" si="2">CONCATENATE("beetle",A3,"-head")</f>
+        <v>beetle2-head</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>Beetle Head 3</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="1"/>
+        <v>A Beetle Head 3</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="2"/>
+        <v>beetle3-head</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>Beetle Head 4</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="1"/>
+        <v>A Beetle Head 4</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="2"/>
+        <v>beetle4-head</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <v>-1</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C1:C1048576"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -535,7 +809,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -557,24 +831,144 @@
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2" t="str">
+        <f t="shared" ref="B2:B5" si="0">CONCATENATE("Beetle Thorax ",A2)</f>
+        <v>Beetle Thorax 1</v>
+      </c>
+      <c r="C2" t="str">
+        <f>CONCATENATE("A ", B2)</f>
+        <v>A Beetle Thorax 1</v>
+      </c>
+      <c r="D2" t="str">
+        <f t="shared" ref="D2:D5" si="1">CONCATENATE("beetle",A2,"-thorax")</f>
+        <v>beetle1-thorax</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" si="0"/>
+        <v>Beetle Thorax 2</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C5" si="2">CONCATENATE("A ", B3)</f>
+        <v>A Beetle Thorax 2</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" si="1"/>
+        <v>beetle2-thorax</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>Beetle Thorax 3</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="2"/>
+        <v>A Beetle Thorax 3</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="1"/>
+        <v>beetle3-thorax</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>Beetle Thorax 4</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="2"/>
+        <v>A Beetle Thorax 4</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="1"/>
+        <v>beetle4-thorax</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>-1</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
-    <col min="2" max="3" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -585,7 +979,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -607,23 +1001,145 @@
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2" t="str">
+        <f t="shared" ref="B2:B5" si="0">CONCATENATE("Beetle Abdomen ",A2)</f>
+        <v>Beetle Abdomen 1</v>
+      </c>
+      <c r="C2" t="str">
+        <f>CONCATENATE("A ", B2)</f>
+        <v>A Beetle Abdomen 1</v>
+      </c>
+      <c r="D2" t="str">
+        <f t="shared" ref="D2:D5" si="1">CONCATENATE("beetle",A2,"-abdomen")</f>
+        <v>beetle1-abdomen</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" si="0"/>
+        <v>Beetle Abdomen 2</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C5" si="2">CONCATENATE("A ", B3)</f>
+        <v>A Beetle Abdomen 2</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" si="1"/>
+        <v>beetle2-abdomen</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>-1</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>Beetle Abdomen 3</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="2"/>
+        <v>A Beetle Abdomen 3</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="1"/>
+        <v>beetle3-abdomen</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>Beetle Abdomen 4</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="2"/>
+        <v>A Beetle Abdomen 4</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="1"/>
+        <v>beetle4-abdomen</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="4" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -656,8 +1172,122 @@
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2" t="str">
+        <f t="shared" ref="B2:B5" si="0">CONCATENATE("Beetle Leg ",A2)</f>
+        <v>Beetle Leg 1</v>
+      </c>
+      <c r="C2" t="str">
+        <f>CONCATENATE("A ", B2)</f>
+        <v>A Beetle Leg 1</v>
+      </c>
+      <c r="D2" t="str">
+        <f t="shared" ref="D2:D5" si="1">CONCATENATE("beetle",A2,)</f>
+        <v>beetle1</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" si="0"/>
+        <v>Beetle Leg 2</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C5" si="2">CONCATENATE("A ", B3)</f>
+        <v>A Beetle Leg 2</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" si="1"/>
+        <v>beetle2</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>Beetle Leg 3</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="2"/>
+        <v>A Beetle Leg 3</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="1"/>
+        <v>beetle3</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>Beetle Leg 4</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="2"/>
+        <v>A Beetle Leg 4</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="1"/>
+        <v>beetle4</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
revised to have base values included
</commit_message>
<xml_diff>
--- a/UnityProject/LD35/Assets/StaticDefinitions/BodyPartDefs.xlsx
+++ b/UnityProject/LD35/Assets/StaticDefinitions/BodyPartDefs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="1320" windowWidth="22035" windowHeight="9285"/>
+    <workbookView xWindow="120" yWindow="1320" windowWidth="22035" windowHeight="9285" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="HeadPartDefs" sheetId="5" r:id="rId1"/>
@@ -158,12 +158,6 @@
   </cellStyles>
   <dxfs count="15">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -185,6 +179,35 @@
         <patternFill patternType="solid">
           <fgColor theme="0" tint="-0.14999847407452621"/>
           <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -222,29 +245,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -318,7 +318,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TabHeadParts" displayName="TabHeadParts" ref="A1:K10" totalsRowShown="0" headerRowDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TabHeadParts" displayName="TabHeadParts" ref="A1:K10" totalsRowShown="0" headerRowDxfId="14">
   <autoFilter ref="A1:K10"/>
   <tableColumns count="11">
     <tableColumn id="1" name="ID"/>
@@ -335,9 +335,9 @@
     <tableColumn id="6" name="damage"/>
     <tableColumn id="7" name="turnSpeed"/>
     <tableColumn id="8" name="jumpForce"/>
-    <tableColumn id="9" name="backSpeed" dataDxfId="7"/>
+    <tableColumn id="9" name="backSpeed" dataDxfId="13"/>
     <tableColumn id="10" name="jumpCooldown"/>
-    <tableColumn id="11" name="VALUE" dataDxfId="1">
+    <tableColumn id="11" name="VALUE" dataDxfId="12">
       <calculatedColumnFormula>TabHeadParts[[#This Row],[health]]/4+TabHeadParts[[#This Row],[damage]]/4+TabHeadParts[[#This Row],[turnSpeed]]/60+TabHeadParts[[#This Row],[jumpForce]]/100+TabHeadParts[[#This Row],[backSpeed]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -346,17 +346,17 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TabThoraxParts" displayName="TabThoraxParts" ref="A1:K10" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TabThoraxParts" displayName="TabThoraxParts" ref="A1:K10" totalsRowShown="0" headerRowDxfId="11">
   <autoFilter ref="A1:K10"/>
   <tableColumns count="11">
     <tableColumn id="1" name="ID"/>
-    <tableColumn id="2" name="name" dataDxfId="5">
+    <tableColumn id="2" name="name" dataDxfId="10">
       <calculatedColumnFormula>CONCATENATE("Beetle Thorax ",A2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="description">
       <calculatedColumnFormula>CONCATENATE("A ", B2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="assetName" dataDxfId="4">
+    <tableColumn id="4" name="assetName" dataDxfId="9">
       <calculatedColumnFormula>CONCATENATE("beetle",A2,"-thorax")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" name="health"/>
@@ -365,7 +365,7 @@
     <tableColumn id="8" name="jumpForce"/>
     <tableColumn id="9" name="backSpeed"/>
     <tableColumn id="10" name="jumpCooldown"/>
-    <tableColumn id="11" name="VALUE" dataDxfId="3">
+    <tableColumn id="11" name="VALUE" dataDxfId="8">
       <calculatedColumnFormula>TabThoraxParts[[#This Row],[health]]/4+TabThoraxParts[[#This Row],[damage]]/2+TabThoraxParts[[#This Row],[turnSpeed]]+TabThoraxParts[[#This Row],[jumpForce]]/200+TabThoraxParts[[#This Row],[backSpeed]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -374,17 +374,17 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="TabAbdomenParts" displayName="TabAbdomenParts" ref="A1:K10" totalsRowShown="0" headerRowDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="TabAbdomenParts" displayName="TabAbdomenParts" ref="A1:K10" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="A1:K10"/>
   <tableColumns count="11">
     <tableColumn id="1" name="ID"/>
-    <tableColumn id="2" name="name" dataDxfId="13">
+    <tableColumn id="2" name="name" dataDxfId="6">
       <calculatedColumnFormula>CONCATENATE("Beetle Abdomen ",A2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="description">
       <calculatedColumnFormula>CONCATENATE("A ", B2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="assetName" dataDxfId="12">
+    <tableColumn id="4" name="assetName" dataDxfId="5">
       <calculatedColumnFormula>CONCATENATE("beetle",A2,"-abdomen")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" name="health"/>
@@ -393,7 +393,7 @@
     <tableColumn id="8" name="jumpForce"/>
     <tableColumn id="9" name="backSpeed"/>
     <tableColumn id="10" name="jumpCooldown"/>
-    <tableColumn id="11" name="VALUE" dataDxfId="0">
+    <tableColumn id="11" name="VALUE" dataDxfId="4">
       <calculatedColumnFormula>TabAbdomenParts[[#This Row],[health]]/4+TabAbdomenParts[[#This Row],[damage]]/2+TabAbdomenParts[[#This Row],[turnSpeed]]+TabAbdomenParts[[#This Row],[jumpForce]]/200+TabAbdomenParts[[#This Row],[backSpeed]]/30</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -402,17 +402,17 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="TabLegParts" displayName="TabLegParts" ref="A1:K6" totalsRowShown="0" headerRowDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="TabLegParts" displayName="TabLegParts" ref="A1:K6" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A1:K6"/>
   <tableColumns count="11">
     <tableColumn id="1" name="ID"/>
-    <tableColumn id="2" name="name" dataDxfId="10">
+    <tableColumn id="2" name="name" dataDxfId="2">
       <calculatedColumnFormula>CONCATENATE("Beetle Leg ",A2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="description">
       <calculatedColumnFormula>CONCATENATE("A ", B2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="assetName" dataDxfId="9">
+    <tableColumn id="4" name="assetName" dataDxfId="1">
       <calculatedColumnFormula>CONCATENATE("beetle",A2,)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" name="health"/>
@@ -421,7 +421,7 @@
     <tableColumn id="8" name="jumpForce"/>
     <tableColumn id="9" name="backSpeed"/>
     <tableColumn id="10" name="jumpCooldown"/>
-    <tableColumn id="11" name="VALUE" dataDxfId="2">
+    <tableColumn id="11" name="VALUE" dataDxfId="0">
       <calculatedColumnFormula>TabLegParts[[#This Row],[health]]/4+TabLegParts[[#This Row],[damage]]/2+TabLegParts[[#This Row],[turnSpeed]]/60+TabLegParts[[#This Row],[jumpForce]]/200+TabLegParts[[#This Row],[backSpeed]]/60</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -752,8 +752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -828,7 +828,7 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G2">
         <v>180</v>
@@ -844,7 +844,7 @@
       </c>
       <c r="K2">
         <f>TabHeadParts[[#This Row],[health]]/4+TabHeadParts[[#This Row],[damage]]/4+TabHeadParts[[#This Row],[turnSpeed]]/60+TabHeadParts[[#This Row],[jumpForce]]/100+TabHeadParts[[#This Row],[backSpeed]]</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -867,7 +867,7 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G3">
         <v>240</v>
@@ -883,7 +883,7 @@
       </c>
       <c r="K3">
         <f>TabHeadParts[[#This Row],[health]]/4+TabHeadParts[[#This Row],[damage]]/4+TabHeadParts[[#This Row],[turnSpeed]]/60+TabHeadParts[[#This Row],[jumpForce]]/100+TabHeadParts[[#This Row],[backSpeed]]</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -906,7 +906,7 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="G4">
         <v>120</v>
@@ -922,7 +922,7 @@
       </c>
       <c r="K4">
         <f>TabHeadParts[[#This Row],[health]]/4+TabHeadParts[[#This Row],[damage]]/4+TabHeadParts[[#This Row],[turnSpeed]]/60+TabHeadParts[[#This Row],[jumpForce]]/100+TabHeadParts[[#This Row],[backSpeed]]</f>
-        <v>5</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -945,7 +945,7 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -961,7 +961,7 @@
       </c>
       <c r="K5">
         <f>TabHeadParts[[#This Row],[health]]/4+TabHeadParts[[#This Row],[damage]]/4+TabHeadParts[[#This Row],[turnSpeed]]/60+TabHeadParts[[#This Row],[jumpForce]]/100+TabHeadParts[[#This Row],[backSpeed]]</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -984,7 +984,7 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G6">
         <v>150</v>
@@ -1000,7 +1000,7 @@
       </c>
       <c r="K6">
         <f>TabHeadParts[[#This Row],[health]]/4+TabHeadParts[[#This Row],[damage]]/4+TabHeadParts[[#This Row],[turnSpeed]]/60+TabHeadParts[[#This Row],[jumpForce]]/100+TabHeadParts[[#This Row],[backSpeed]]</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1023,7 +1023,7 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G7">
         <v>120</v>
@@ -1039,7 +1039,7 @@
       </c>
       <c r="K7">
         <f>TabHeadParts[[#This Row],[health]]/4+TabHeadParts[[#This Row],[damage]]/4+TabHeadParts[[#This Row],[turnSpeed]]/60+TabHeadParts[[#This Row],[jumpForce]]/100+TabHeadParts[[#This Row],[backSpeed]]</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1062,7 +1062,7 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G8">
         <v>60</v>
@@ -1078,7 +1078,7 @@
       </c>
       <c r="K8">
         <f>TabHeadParts[[#This Row],[health]]/4+TabHeadParts[[#This Row],[damage]]/4+TabHeadParts[[#This Row],[turnSpeed]]/60+TabHeadParts[[#This Row],[jumpForce]]/100+TabHeadParts[[#This Row],[backSpeed]]</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1101,7 +1101,7 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -1117,7 +1117,7 @@
       </c>
       <c r="K9">
         <f>TabHeadParts[[#This Row],[health]]/4+TabHeadParts[[#This Row],[damage]]/4+TabHeadParts[[#This Row],[turnSpeed]]/60+TabHeadParts[[#This Row],[jumpForce]]/100+TabHeadParts[[#This Row],[backSpeed]]</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1140,7 +1140,7 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G10">
         <v>120</v>
@@ -1156,7 +1156,7 @@
       </c>
       <c r="K10">
         <f>TabHeadParts[[#This Row],[health]]/4+TabHeadParts[[#This Row],[damage]]/4+TabHeadParts[[#This Row],[turnSpeed]]/60+TabHeadParts[[#This Row],[jumpForce]]/100+TabHeadParts[[#This Row],[backSpeed]]</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1172,8 +1172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1251,17 +1251,17 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>600</v>
+        <v>1200</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K2">
         <f>TabThoraxParts[[#This Row],[health]]/4+TabThoraxParts[[#This Row],[damage]]/2+TabThoraxParts[[#This Row],[turnSpeed]]+TabThoraxParts[[#This Row],[jumpForce]]/200+TabThoraxParts[[#This Row],[backSpeed]]</f>
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1290,17 +1290,17 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="I3">
         <v>0</v>
       </c>
       <c r="J3">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="K3">
         <f>TabThoraxParts[[#This Row],[health]]/4+TabThoraxParts[[#This Row],[damage]]/2+TabThoraxParts[[#This Row],[turnSpeed]]+TabThoraxParts[[#This Row],[jumpForce]]/200+TabThoraxParts[[#This Row],[backSpeed]]</f>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1329,17 +1329,17 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <v>100</v>
+        <v>700</v>
       </c>
       <c r="I4">
         <v>0</v>
       </c>
       <c r="J4">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="K4">
         <f>TabThoraxParts[[#This Row],[health]]/4+TabThoraxParts[[#This Row],[damage]]/2+TabThoraxParts[[#This Row],[turnSpeed]]+TabThoraxParts[[#This Row],[jumpForce]]/200+TabThoraxParts[[#This Row],[backSpeed]]</f>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1368,17 +1368,17 @@
         <v>0</v>
       </c>
       <c r="H5">
-        <v>400</v>
+        <v>1000</v>
       </c>
       <c r="I5">
         <v>0</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K5">
         <f>TabThoraxParts[[#This Row],[health]]/4+TabThoraxParts[[#This Row],[damage]]/2+TabThoraxParts[[#This Row],[turnSpeed]]+TabThoraxParts[[#This Row],[jumpForce]]/200+TabThoraxParts[[#This Row],[backSpeed]]</f>
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1407,17 +1407,17 @@
         <v>0</v>
       </c>
       <c r="H6">
-        <v>800</v>
+        <v>1400</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K6">
         <f>TabThoraxParts[[#This Row],[health]]/4+TabThoraxParts[[#This Row],[damage]]/2+TabThoraxParts[[#This Row],[turnSpeed]]+TabThoraxParts[[#This Row],[jumpForce]]/200+TabThoraxParts[[#This Row],[backSpeed]]</f>
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1446,17 +1446,17 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <v>400</v>
+        <v>1000</v>
       </c>
       <c r="I7">
         <v>0</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K7">
         <f>TabThoraxParts[[#This Row],[health]]/4+TabThoraxParts[[#This Row],[damage]]/2+TabThoraxParts[[#This Row],[turnSpeed]]+TabThoraxParts[[#This Row],[jumpForce]]/200+TabThoraxParts[[#This Row],[backSpeed]]</f>
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1485,17 +1485,17 @@
         <v>0</v>
       </c>
       <c r="H8">
-        <v>300</v>
+        <v>900</v>
       </c>
       <c r="I8">
         <v>0</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K8">
         <f>TabThoraxParts[[#This Row],[health]]/4+TabThoraxParts[[#This Row],[damage]]/2+TabThoraxParts[[#This Row],[turnSpeed]]+TabThoraxParts[[#This Row],[jumpForce]]/200+TabThoraxParts[[#This Row],[backSpeed]]</f>
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1524,17 +1524,17 @@
         <v>0</v>
       </c>
       <c r="H9">
-        <v>200</v>
+        <v>800</v>
       </c>
       <c r="I9">
         <v>0</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K9">
         <f>TabThoraxParts[[#This Row],[health]]/4+TabThoraxParts[[#This Row],[damage]]/2+TabThoraxParts[[#This Row],[turnSpeed]]+TabThoraxParts[[#This Row],[jumpForce]]/200+TabThoraxParts[[#This Row],[backSpeed]]</f>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1563,17 +1563,17 @@
         <v>0</v>
       </c>
       <c r="H10">
-        <v>500</v>
+        <v>1100</v>
       </c>
       <c r="I10">
         <v>0</v>
       </c>
       <c r="J10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K10">
         <f>TabThoraxParts[[#This Row],[health]]/4+TabThoraxParts[[#This Row],[damage]]/2+TabThoraxParts[[#This Row],[turnSpeed]]+TabThoraxParts[[#This Row],[jumpForce]]/200+TabThoraxParts[[#This Row],[backSpeed]]</f>
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1589,7 +1589,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1658,7 +1658,7 @@
         <v>beetle1-abdomen</v>
       </c>
       <c r="E2">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -1677,7 +1677,7 @@
       </c>
       <c r="K2">
         <f>TabAbdomenParts[[#This Row],[health]]/4+TabAbdomenParts[[#This Row],[damage]]/2+TabAbdomenParts[[#This Row],[turnSpeed]]+TabAbdomenParts[[#This Row],[jumpForce]]/200+TabAbdomenParts[[#This Row],[backSpeed]]/30</f>
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1697,7 +1697,7 @@
         <v>beetle2-abdomen</v>
       </c>
       <c r="E3">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1716,7 +1716,7 @@
       </c>
       <c r="K3">
         <f>TabAbdomenParts[[#This Row],[health]]/4+TabAbdomenParts[[#This Row],[damage]]/2+TabAbdomenParts[[#This Row],[turnSpeed]]+TabAbdomenParts[[#This Row],[jumpForce]]/200+TabAbdomenParts[[#This Row],[backSpeed]]/30</f>
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1736,7 +1736,7 @@
         <v>beetle3-abdomen</v>
       </c>
       <c r="E4">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -1755,7 +1755,7 @@
       </c>
       <c r="K4">
         <f>TabAbdomenParts[[#This Row],[health]]/4+TabAbdomenParts[[#This Row],[damage]]/2+TabAbdomenParts[[#This Row],[turnSpeed]]+TabAbdomenParts[[#This Row],[jumpForce]]/200+TabAbdomenParts[[#This Row],[backSpeed]]/30</f>
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1775,7 +1775,7 @@
         <v>beetle4-abdomen</v>
       </c>
       <c r="E5">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -1794,7 +1794,7 @@
       </c>
       <c r="K5">
         <f>TabAbdomenParts[[#This Row],[health]]/4+TabAbdomenParts[[#This Row],[damage]]/2+TabAbdomenParts[[#This Row],[turnSpeed]]+TabAbdomenParts[[#This Row],[jumpForce]]/200+TabAbdomenParts[[#This Row],[backSpeed]]/30</f>
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1814,7 +1814,7 @@
         <v>beetle5-abdomen</v>
       </c>
       <c r="E6">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -1833,7 +1833,7 @@
       </c>
       <c r="K6">
         <f>TabAbdomenParts[[#This Row],[health]]/4+TabAbdomenParts[[#This Row],[damage]]/2+TabAbdomenParts[[#This Row],[turnSpeed]]+TabAbdomenParts[[#This Row],[jumpForce]]/200+TabAbdomenParts[[#This Row],[backSpeed]]/30</f>
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1853,7 +1853,7 @@
         <v>beetle6-abdomen</v>
       </c>
       <c r="E7">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -1872,7 +1872,7 @@
       </c>
       <c r="K7">
         <f>TabAbdomenParts[[#This Row],[health]]/4+TabAbdomenParts[[#This Row],[damage]]/2+TabAbdomenParts[[#This Row],[turnSpeed]]+TabAbdomenParts[[#This Row],[jumpForce]]/200+TabAbdomenParts[[#This Row],[backSpeed]]/30</f>
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1892,7 +1892,7 @@
         <v>beetle7-abdomen</v>
       </c>
       <c r="E8">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -1911,7 +1911,7 @@
       </c>
       <c r="K8">
         <f>TabAbdomenParts[[#This Row],[health]]/4+TabAbdomenParts[[#This Row],[damage]]/2+TabAbdomenParts[[#This Row],[turnSpeed]]+TabAbdomenParts[[#This Row],[jumpForce]]/200+TabAbdomenParts[[#This Row],[backSpeed]]/30</f>
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1931,7 +1931,7 @@
         <v>beetle8-abdomen</v>
       </c>
       <c r="E9">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -1950,7 +1950,7 @@
       </c>
       <c r="K9">
         <f>TabAbdomenParts[[#This Row],[health]]/4+TabAbdomenParts[[#This Row],[damage]]/2+TabAbdomenParts[[#This Row],[turnSpeed]]+TabAbdomenParts[[#This Row],[jumpForce]]/200+TabAbdomenParts[[#This Row],[backSpeed]]/30</f>
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1970,7 +1970,7 @@
         <v>beetle9-abdomen</v>
       </c>
       <c r="E10">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -1989,7 +1989,7 @@
       </c>
       <c r="K10">
         <f>TabAbdomenParts[[#This Row],[health]]/4+TabAbdomenParts[[#This Row],[damage]]/2+TabAbdomenParts[[#This Row],[turnSpeed]]+TabAbdomenParts[[#This Row],[jumpForce]]/200+TabAbdomenParts[[#This Row],[backSpeed]]/30</f>
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -2006,7 +2006,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2081,20 +2081,20 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>240</v>
+        <v>360</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="J2">
         <v>0</v>
       </c>
       <c r="K2" s="2">
         <f>TabLegParts[[#This Row],[health]]/4+TabLegParts[[#This Row],[damage]]/2+TabLegParts[[#This Row],[turnSpeed]]/60+TabLegParts[[#This Row],[jumpForce]]/200+TabLegParts[[#This Row],[backSpeed]]/60</f>
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -2120,20 +2120,20 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>90</v>
+        <v>210</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="J3">
         <v>0</v>
       </c>
       <c r="K3" s="3">
         <f>TabLegParts[[#This Row],[health]]/4+TabLegParts[[#This Row],[damage]]/2+TabLegParts[[#This Row],[turnSpeed]]/60+TabLegParts[[#This Row],[jumpForce]]/200+TabLegParts[[#This Row],[backSpeed]]/60</f>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -2159,20 +2159,20 @@
         <v>0</v>
       </c>
       <c r="G4">
+        <v>240</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
         <v>120</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>60</v>
       </c>
       <c r="J4">
         <v>0</v>
       </c>
       <c r="K4" s="2">
         <f>TabLegParts[[#This Row],[health]]/4+TabLegParts[[#This Row],[damage]]/2+TabLegParts[[#This Row],[turnSpeed]]/60+TabLegParts[[#This Row],[jumpForce]]/200+TabLegParts[[#This Row],[backSpeed]]/60</f>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -2198,20 +2198,20 @@
         <v>0</v>
       </c>
       <c r="G5">
+        <v>300</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
         <v>180</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>120</v>
       </c>
       <c r="J5">
         <v>0</v>
       </c>
       <c r="K5" s="3">
         <f>TabLegParts[[#This Row],[health]]/4+TabLegParts[[#This Row],[damage]]/2+TabLegParts[[#This Row],[turnSpeed]]/60+TabLegParts[[#This Row],[jumpForce]]/200+TabLegParts[[#This Row],[backSpeed]]/60</f>
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -2237,20 +2237,20 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>60</v>
+        <v>180</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
-        <v>180</v>
+        <v>240</v>
       </c>
       <c r="J6">
         <v>0</v>
       </c>
       <c r="K6" s="2">
         <f>TabLegParts[[#This Row],[health]]/4+TabLegParts[[#This Row],[damage]]/2+TabLegParts[[#This Row],[turnSpeed]]/60+TabLegParts[[#This Row],[jumpForce]]/200+TabLegParts[[#This Row],[backSpeed]]/60</f>
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding Border.prefab, adding border to scene, and lowering some jump cooldowns
</commit_message>
<xml_diff>
--- a/UnityProject/LD35/Assets/StaticDefinitions/BodyPartDefs.xlsx
+++ b/UnityProject/LD35/Assets/StaticDefinitions/BodyPartDefs.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UnityProjects\ld35-master\UnityProject\LD35\Assets\StaticDefinitions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LD35\trunk\UnityProject\LD35\Assets\StaticDefinitions\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="1320" windowWidth="22035" windowHeight="9285" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="1920" windowWidth="22035" windowHeight="9285" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="HeadPartDefs" sheetId="5" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="AbdomenPartDefs" sheetId="3" r:id="rId3"/>
     <sheet name="LegPartDefs" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -171,7 +171,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -505,23 +504,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -557,23 +539,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1173,7 +1138,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1257,7 +1222,7 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K2">
         <f>TabThoraxParts[[#This Row],[health]]/4+TabThoraxParts[[#This Row],[damage]]/2+TabThoraxParts[[#This Row],[turnSpeed]]+TabThoraxParts[[#This Row],[jumpForce]]/200+TabThoraxParts[[#This Row],[backSpeed]]</f>
@@ -1296,7 +1261,7 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K3">
         <f>TabThoraxParts[[#This Row],[health]]/4+TabThoraxParts[[#This Row],[damage]]/2+TabThoraxParts[[#This Row],[turnSpeed]]+TabThoraxParts[[#This Row],[jumpForce]]/200+TabThoraxParts[[#This Row],[backSpeed]]</f>
@@ -1335,7 +1300,7 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K4">
         <f>TabThoraxParts[[#This Row],[health]]/4+TabThoraxParts[[#This Row],[damage]]/2+TabThoraxParts[[#This Row],[turnSpeed]]+TabThoraxParts[[#This Row],[jumpForce]]/200+TabThoraxParts[[#This Row],[backSpeed]]</f>
@@ -1374,7 +1339,7 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K5">
         <f>TabThoraxParts[[#This Row],[health]]/4+TabThoraxParts[[#This Row],[damage]]/2+TabThoraxParts[[#This Row],[turnSpeed]]+TabThoraxParts[[#This Row],[jumpForce]]/200+TabThoraxParts[[#This Row],[backSpeed]]</f>
@@ -1413,7 +1378,7 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K6">
         <f>TabThoraxParts[[#This Row],[health]]/4+TabThoraxParts[[#This Row],[damage]]/2+TabThoraxParts[[#This Row],[turnSpeed]]+TabThoraxParts[[#This Row],[jumpForce]]/200+TabThoraxParts[[#This Row],[backSpeed]]</f>
@@ -1452,7 +1417,7 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K7">
         <f>TabThoraxParts[[#This Row],[health]]/4+TabThoraxParts[[#This Row],[damage]]/2+TabThoraxParts[[#This Row],[turnSpeed]]+TabThoraxParts[[#This Row],[jumpForce]]/200+TabThoraxParts[[#This Row],[backSpeed]]</f>
@@ -1491,7 +1456,7 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K8">
         <f>TabThoraxParts[[#This Row],[health]]/4+TabThoraxParts[[#This Row],[damage]]/2+TabThoraxParts[[#This Row],[turnSpeed]]+TabThoraxParts[[#This Row],[jumpForce]]/200+TabThoraxParts[[#This Row],[backSpeed]]</f>
@@ -1530,7 +1495,7 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K9">
         <f>TabThoraxParts[[#This Row],[health]]/4+TabThoraxParts[[#This Row],[damage]]/2+TabThoraxParts[[#This Row],[turnSpeed]]+TabThoraxParts[[#This Row],[jumpForce]]/200+TabThoraxParts[[#This Row],[backSpeed]]</f>
@@ -1569,7 +1534,7 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K10">
         <f>TabThoraxParts[[#This Row],[health]]/4+TabThoraxParts[[#This Row],[damage]]/2+TabThoraxParts[[#This Row],[turnSpeed]]+TabThoraxParts[[#This Row],[jumpForce]]/200+TabThoraxParts[[#This Row],[backSpeed]]</f>
@@ -1589,7 +1554,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2006,7 +1971,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
new actually kinda balanced data
</commit_message>
<xml_diff>
--- a/UnityProject/LD35/Assets/StaticDefinitions/BodyPartDefs.xlsx
+++ b/UnityProject/LD35/Assets/StaticDefinitions/BodyPartDefs.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LD35\trunk\UnityProject\LD35\Assets\StaticDefinitions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UnityProjects\ld35-master\UnityProject\LD35\Assets\StaticDefinitions\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="1920" windowWidth="22035" windowHeight="9285" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="1920" windowWidth="22035" windowHeight="9285"/>
   </bookViews>
   <sheets>
     <sheet name="HeadPartDefs" sheetId="5" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="AbdomenPartDefs" sheetId="3" r:id="rId3"/>
     <sheet name="LegPartDefs" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -504,6 +504,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -539,6 +556,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -717,8 +751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -796,7 +830,7 @@
         <v>8</v>
       </c>
       <c r="G2">
-        <v>180</v>
+        <v>60</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -809,7 +843,7 @@
       </c>
       <c r="K2">
         <f>TabHeadParts[[#This Row],[health]]/4+TabHeadParts[[#This Row],[damage]]/4+TabHeadParts[[#This Row],[turnSpeed]]/60+TabHeadParts[[#This Row],[jumpForce]]/100+TabHeadParts[[#This Row],[backSpeed]]</f>
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -835,7 +869,7 @@
         <v>8</v>
       </c>
       <c r="G3">
-        <v>240</v>
+        <v>80</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -848,7 +882,7 @@
       </c>
       <c r="K3">
         <f>TabHeadParts[[#This Row],[health]]/4+TabHeadParts[[#This Row],[damage]]/4+TabHeadParts[[#This Row],[turnSpeed]]/60+TabHeadParts[[#This Row],[jumpForce]]/100+TabHeadParts[[#This Row],[backSpeed]]</f>
-        <v>6</v>
+        <v>3.333333333333333</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -874,7 +908,7 @@
         <v>18</v>
       </c>
       <c r="G4">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -887,7 +921,7 @@
       </c>
       <c r="K4">
         <f>TabHeadParts[[#This Row],[health]]/4+TabHeadParts[[#This Row],[damage]]/4+TabHeadParts[[#This Row],[turnSpeed]]/60+TabHeadParts[[#This Row],[jumpForce]]/100+TabHeadParts[[#This Row],[backSpeed]]</f>
-        <v>6.5</v>
+        <v>5.166666666666667</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -952,7 +986,7 @@
         <v>6</v>
       </c>
       <c r="G6">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -965,7 +999,7 @@
       </c>
       <c r="K6">
         <f>TabHeadParts[[#This Row],[health]]/4+TabHeadParts[[#This Row],[damage]]/4+TabHeadParts[[#This Row],[turnSpeed]]/60+TabHeadParts[[#This Row],[jumpForce]]/100+TabHeadParts[[#This Row],[backSpeed]]</f>
-        <v>4</v>
+        <v>2.3333333333333335</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -991,7 +1025,7 @@
         <v>8</v>
       </c>
       <c r="G7">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -1004,7 +1038,7 @@
       </c>
       <c r="K7">
         <f>TabHeadParts[[#This Row],[health]]/4+TabHeadParts[[#This Row],[damage]]/4+TabHeadParts[[#This Row],[turnSpeed]]/60+TabHeadParts[[#This Row],[jumpForce]]/100+TabHeadParts[[#This Row],[backSpeed]]</f>
-        <v>4</v>
+        <v>2.6666666666666665</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1030,7 +1064,7 @@
         <v>12</v>
       </c>
       <c r="G8">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -1043,7 +1077,7 @@
       </c>
       <c r="K8">
         <f>TabHeadParts[[#This Row],[health]]/4+TabHeadParts[[#This Row],[damage]]/4+TabHeadParts[[#This Row],[turnSpeed]]/60+TabHeadParts[[#This Row],[jumpForce]]/100+TabHeadParts[[#This Row],[backSpeed]]</f>
-        <v>4</v>
+        <v>3.3333333333333335</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1108,7 +1142,7 @@
         <v>12</v>
       </c>
       <c r="G10">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -1121,7 +1155,7 @@
       </c>
       <c r="K10">
         <f>TabHeadParts[[#This Row],[health]]/4+TabHeadParts[[#This Row],[damage]]/4+TabHeadParts[[#This Row],[turnSpeed]]/60+TabHeadParts[[#This Row],[jumpForce]]/100+TabHeadParts[[#This Row],[backSpeed]]</f>
-        <v>5</v>
+        <v>3.6666666666666665</v>
       </c>
     </row>
   </sheetData>
@@ -1137,8 +1171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1216,17 +1250,17 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>1200</v>
+        <v>1300</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>1.7</v>
       </c>
       <c r="K2">
         <f>TabThoraxParts[[#This Row],[health]]/4+TabThoraxParts[[#This Row],[damage]]/2+TabThoraxParts[[#This Row],[turnSpeed]]+TabThoraxParts[[#This Row],[jumpForce]]/200+TabThoraxParts[[#This Row],[backSpeed]]</f>
-        <v>8</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1255,17 +1289,17 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>600</v>
+        <v>700</v>
       </c>
       <c r="I3">
         <v>0</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="K3">
         <f>TabThoraxParts[[#This Row],[health]]/4+TabThoraxParts[[#This Row],[damage]]/2+TabThoraxParts[[#This Row],[turnSpeed]]+TabThoraxParts[[#This Row],[jumpForce]]/200+TabThoraxParts[[#This Row],[backSpeed]]</f>
-        <v>6</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1294,17 +1328,17 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="I4">
         <v>0</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="K4">
         <f>TabThoraxParts[[#This Row],[health]]/4+TabThoraxParts[[#This Row],[damage]]/2+TabThoraxParts[[#This Row],[turnSpeed]]+TabThoraxParts[[#This Row],[jumpForce]]/200+TabThoraxParts[[#This Row],[backSpeed]]</f>
-        <v>6</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1333,17 +1367,17 @@
         <v>0</v>
       </c>
       <c r="H5">
-        <v>1000</v>
+        <v>1100</v>
       </c>
       <c r="I5">
         <v>0</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="K5">
         <f>TabThoraxParts[[#This Row],[health]]/4+TabThoraxParts[[#This Row],[damage]]/2+TabThoraxParts[[#This Row],[turnSpeed]]+TabThoraxParts[[#This Row],[jumpForce]]/200+TabThoraxParts[[#This Row],[backSpeed]]</f>
-        <v>7</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1372,17 +1406,17 @@
         <v>0</v>
       </c>
       <c r="H6">
-        <v>1400</v>
+        <v>1500</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6">
-        <v>1</v>
+        <v>1.8</v>
       </c>
       <c r="K6">
         <f>TabThoraxParts[[#This Row],[health]]/4+TabThoraxParts[[#This Row],[damage]]/2+TabThoraxParts[[#This Row],[turnSpeed]]+TabThoraxParts[[#This Row],[jumpForce]]/200+TabThoraxParts[[#This Row],[backSpeed]]</f>
-        <v>8</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1411,17 +1445,17 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <v>1000</v>
+        <v>1100</v>
       </c>
       <c r="I7">
         <v>0</v>
       </c>
       <c r="J7">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="K7">
         <f>TabThoraxParts[[#This Row],[health]]/4+TabThoraxParts[[#This Row],[damage]]/2+TabThoraxParts[[#This Row],[turnSpeed]]+TabThoraxParts[[#This Row],[jumpForce]]/200+TabThoraxParts[[#This Row],[backSpeed]]</f>
-        <v>8</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1450,17 +1484,17 @@
         <v>0</v>
       </c>
       <c r="H8">
-        <v>900</v>
+        <v>1100</v>
       </c>
       <c r="I8">
         <v>0</v>
       </c>
       <c r="J8">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="K8">
         <f>TabThoraxParts[[#This Row],[health]]/4+TabThoraxParts[[#This Row],[damage]]/2+TabThoraxParts[[#This Row],[turnSpeed]]+TabThoraxParts[[#This Row],[jumpForce]]/200+TabThoraxParts[[#This Row],[backSpeed]]</f>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1489,7 +1523,7 @@
         <v>0</v>
       </c>
       <c r="H9">
-        <v>800</v>
+        <v>900</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -1499,7 +1533,7 @@
       </c>
       <c r="K9">
         <f>TabThoraxParts[[#This Row],[health]]/4+TabThoraxParts[[#This Row],[damage]]/2+TabThoraxParts[[#This Row],[turnSpeed]]+TabThoraxParts[[#This Row],[jumpForce]]/200+TabThoraxParts[[#This Row],[backSpeed]]</f>
-        <v>6</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1528,17 +1562,17 @@
         <v>0</v>
       </c>
       <c r="H10">
-        <v>1100</v>
+        <v>1200</v>
       </c>
       <c r="I10">
         <v>0</v>
       </c>
       <c r="J10">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="K10">
         <f>TabThoraxParts[[#This Row],[health]]/4+TabThoraxParts[[#This Row],[damage]]/2+TabThoraxParts[[#This Row],[turnSpeed]]+TabThoraxParts[[#This Row],[jumpForce]]/200+TabThoraxParts[[#This Row],[backSpeed]]</f>
-        <v>7</v>
+        <v>7.5</v>
       </c>
     </row>
   </sheetData>
@@ -1553,8 +1587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1635,14 +1669,14 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="J2">
         <v>0</v>
       </c>
       <c r="K2">
         <f>TabAbdomenParts[[#This Row],[health]]/4+TabAbdomenParts[[#This Row],[damage]]/2+TabAbdomenParts[[#This Row],[turnSpeed]]+TabAbdomenParts[[#This Row],[jumpForce]]/200+TabAbdomenParts[[#This Row],[backSpeed]]/30</f>
-        <v>10</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1674,14 +1708,14 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="J3">
         <v>0</v>
       </c>
       <c r="K3">
         <f>TabAbdomenParts[[#This Row],[health]]/4+TabAbdomenParts[[#This Row],[damage]]/2+TabAbdomenParts[[#This Row],[turnSpeed]]+TabAbdomenParts[[#This Row],[jumpForce]]/200+TabAbdomenParts[[#This Row],[backSpeed]]/30</f>
-        <v>9</v>
+        <v>8.5666666666666664</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1713,14 +1747,14 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="J4">
         <v>0</v>
       </c>
       <c r="K4">
         <f>TabAbdomenParts[[#This Row],[health]]/4+TabAbdomenParts[[#This Row],[damage]]/2+TabAbdomenParts[[#This Row],[turnSpeed]]+TabAbdomenParts[[#This Row],[jumpForce]]/200+TabAbdomenParts[[#This Row],[backSpeed]]/30</f>
-        <v>9</v>
+        <v>7.2</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1752,14 +1786,14 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="J5">
         <v>0</v>
       </c>
       <c r="K5">
         <f>TabAbdomenParts[[#This Row],[health]]/4+TabAbdomenParts[[#This Row],[damage]]/2+TabAbdomenParts[[#This Row],[turnSpeed]]+TabAbdomenParts[[#This Row],[jumpForce]]/200+TabAbdomenParts[[#This Row],[backSpeed]]/30</f>
-        <v>8</v>
+        <v>7.5666666666666664</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1791,14 +1825,14 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>105</v>
+        <v>1</v>
       </c>
       <c r="J6">
         <v>0</v>
       </c>
       <c r="K6">
         <f>TabAbdomenParts[[#This Row],[health]]/4+TabAbdomenParts[[#This Row],[damage]]/2+TabAbdomenParts[[#This Row],[turnSpeed]]+TabAbdomenParts[[#This Row],[jumpForce]]/200+TabAbdomenParts[[#This Row],[backSpeed]]/30</f>
-        <v>10</v>
+        <v>6.5333333333333332</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1830,14 +1864,14 @@
         <v>0</v>
       </c>
       <c r="I7">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="J7">
         <v>0</v>
       </c>
       <c r="K7">
         <f>TabAbdomenParts[[#This Row],[health]]/4+TabAbdomenParts[[#This Row],[damage]]/2+TabAbdomenParts[[#This Row],[turnSpeed]]+TabAbdomenParts[[#This Row],[jumpForce]]/200+TabAbdomenParts[[#This Row],[backSpeed]]/30</f>
-        <v>9</v>
+        <v>7.6333333333333337</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1869,14 +1903,14 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="J8">
         <v>0</v>
       </c>
       <c r="K8">
         <f>TabAbdomenParts[[#This Row],[health]]/4+TabAbdomenParts[[#This Row],[damage]]/2+TabAbdomenParts[[#This Row],[turnSpeed]]+TabAbdomenParts[[#This Row],[jumpForce]]/200+TabAbdomenParts[[#This Row],[backSpeed]]/30</f>
-        <v>10</v>
+        <v>8.1999999999999993</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1908,14 +1942,14 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="J9">
         <v>0</v>
       </c>
       <c r="K9">
         <f>TabAbdomenParts[[#This Row],[health]]/4+TabAbdomenParts[[#This Row],[damage]]/2+TabAbdomenParts[[#This Row],[turnSpeed]]+TabAbdomenParts[[#This Row],[jumpForce]]/200+TabAbdomenParts[[#This Row],[backSpeed]]/30</f>
-        <v>8</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1947,14 +1981,14 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="J10">
         <v>0</v>
       </c>
       <c r="K10">
         <f>TabAbdomenParts[[#This Row],[health]]/4+TabAbdomenParts[[#This Row],[damage]]/2+TabAbdomenParts[[#This Row],[turnSpeed]]+TabAbdomenParts[[#This Row],[jumpForce]]/200+TabAbdomenParts[[#This Row],[backSpeed]]/30</f>
-        <v>8</v>
+        <v>7.5666666666666664</v>
       </c>
     </row>
   </sheetData>
@@ -1971,7 +2005,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2046,20 +2080,20 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>360</v>
+        <v>120</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
-        <v>60</v>
+        <v>8</v>
       </c>
       <c r="J2">
         <v>0</v>
       </c>
       <c r="K2" s="2">
         <f>TabLegParts[[#This Row],[health]]/4+TabLegParts[[#This Row],[damage]]/2+TabLegParts[[#This Row],[turnSpeed]]/60+TabLegParts[[#This Row],[jumpForce]]/200+TabLegParts[[#This Row],[backSpeed]]/60</f>
-        <v>7</v>
+        <v>2.1333333333333333</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -2085,20 +2119,20 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>210</v>
+        <v>70</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>150</v>
+        <v>10</v>
       </c>
       <c r="J3">
         <v>0</v>
       </c>
       <c r="K3" s="3">
         <f>TabLegParts[[#This Row],[health]]/4+TabLegParts[[#This Row],[damage]]/2+TabLegParts[[#This Row],[turnSpeed]]/60+TabLegParts[[#This Row],[jumpForce]]/200+TabLegParts[[#This Row],[backSpeed]]/60</f>
-        <v>6</v>
+        <v>1.3333333333333335</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -2124,20 +2158,20 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>240</v>
+        <v>80</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4">
-        <v>120</v>
+        <v>4</v>
       </c>
       <c r="J4">
         <v>0</v>
       </c>
       <c r="K4" s="2">
         <f>TabLegParts[[#This Row],[health]]/4+TabLegParts[[#This Row],[damage]]/2+TabLegParts[[#This Row],[turnSpeed]]/60+TabLegParts[[#This Row],[jumpForce]]/200+TabLegParts[[#This Row],[backSpeed]]/60</f>
-        <v>6</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -2163,20 +2197,20 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5">
-        <v>180</v>
+        <v>12</v>
       </c>
       <c r="J5">
         <v>0</v>
       </c>
       <c r="K5" s="3">
         <f>TabLegParts[[#This Row],[health]]/4+TabLegParts[[#This Row],[damage]]/2+TabLegParts[[#This Row],[turnSpeed]]/60+TabLegParts[[#This Row],[jumpForce]]/200+TabLegParts[[#This Row],[backSpeed]]/60</f>
-        <v>8</v>
+        <v>1.8666666666666667</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -2202,20 +2236,20 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>180</v>
+        <v>60</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
-        <v>240</v>
+        <v>16</v>
       </c>
       <c r="J6">
         <v>0</v>
       </c>
       <c r="K6" s="2">
         <f>TabLegParts[[#This Row],[health]]/4+TabLegParts[[#This Row],[damage]]/2+TabLegParts[[#This Row],[turnSpeed]]/60+TabLegParts[[#This Row],[jumpForce]]/200+TabLegParts[[#This Row],[backSpeed]]/60</f>
-        <v>7</v>
+        <v>1.2666666666666666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating balancing, adding clamp to values
</commit_message>
<xml_diff>
--- a/UnityProject/LD35/Assets/StaticDefinitions/BodyPartDefs.xlsx
+++ b/UnityProject/LD35/Assets/StaticDefinitions/BodyPartDefs.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UnityProjects\ld35-master\UnityProject\LD35\Assets\StaticDefinitions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LD35\trunk\UnityProject\LD35\Assets\StaticDefinitions\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="1920" windowWidth="22035" windowHeight="9285"/>
+    <workbookView xWindow="120" yWindow="2520" windowWidth="22035" windowHeight="9285" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="HeadPartDefs" sheetId="5" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="AbdomenPartDefs" sheetId="3" r:id="rId3"/>
     <sheet name="LegPartDefs" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -188,61 +188,6 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -303,6 +248,61 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -319,6 +319,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TabHeadParts" displayName="TabHeadParts" ref="A1:K10" totalsRowShown="0" headerRowDxfId="14">
   <autoFilter ref="A1:K10"/>
+  <sortState ref="A2:K10">
+    <sortCondition ref="G1:G10"/>
+  </sortState>
   <tableColumns count="11">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="name">
@@ -336,8 +339,8 @@
     <tableColumn id="8" name="jumpForce"/>
     <tableColumn id="9" name="backSpeed" dataDxfId="13"/>
     <tableColumn id="10" name="jumpCooldown"/>
-    <tableColumn id="11" name="VALUE" dataDxfId="12">
-      <calculatedColumnFormula>TabHeadParts[[#This Row],[health]]/4+TabHeadParts[[#This Row],[damage]]/4+TabHeadParts[[#This Row],[turnSpeed]]/60+TabHeadParts[[#This Row],[jumpForce]]/100+TabHeadParts[[#This Row],[backSpeed]]</calculatedColumnFormula>
+    <tableColumn id="11" name="VALUE" dataDxfId="3">
+      <calculatedColumnFormula>TabHeadParts[[#This Row],[health]]/50+TabHeadParts[[#This Row],[damage]]/25+TabHeadParts[[#This Row],[turnSpeed]]/160+TabHeadParts[[#This Row],[jumpForce]]/1300+TabHeadParts[[#This Row],[backSpeed]]/25</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -345,17 +348,17 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TabThoraxParts" displayName="TabThoraxParts" ref="A1:K10" totalsRowShown="0" headerRowDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TabThoraxParts" displayName="TabThoraxParts" ref="A1:K10" totalsRowShown="0" headerRowDxfId="12">
   <autoFilter ref="A1:K10"/>
   <tableColumns count="11">
     <tableColumn id="1" name="ID"/>
-    <tableColumn id="2" name="name" dataDxfId="10">
+    <tableColumn id="2" name="name" dataDxfId="11">
       <calculatedColumnFormula>CONCATENATE("Beetle Thorax ",A2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="description">
       <calculatedColumnFormula>CONCATENATE("A ", B2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="assetName" dataDxfId="9">
+    <tableColumn id="4" name="assetName" dataDxfId="10">
       <calculatedColumnFormula>CONCATENATE("beetle",A2,"-thorax")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" name="health"/>
@@ -364,8 +367,8 @@
     <tableColumn id="8" name="jumpForce"/>
     <tableColumn id="9" name="backSpeed"/>
     <tableColumn id="10" name="jumpCooldown"/>
-    <tableColumn id="11" name="VALUE" dataDxfId="8">
-      <calculatedColumnFormula>TabThoraxParts[[#This Row],[health]]/4+TabThoraxParts[[#This Row],[damage]]/2+TabThoraxParts[[#This Row],[turnSpeed]]+TabThoraxParts[[#This Row],[jumpForce]]/200+TabThoraxParts[[#This Row],[backSpeed]]</calculatedColumnFormula>
+    <tableColumn id="11" name="VALUE" dataDxfId="2">
+      <calculatedColumnFormula>TabThoraxParts[[#This Row],[health]]/50+TabThoraxParts[[#This Row],[damage]]/25+TabThoraxParts[[#This Row],[turnSpeed]]/160+TabThoraxParts[[#This Row],[jumpForce]]/1300+TabThoraxParts[[#This Row],[backSpeed]]/25+1/TabThoraxParts[[#This Row],[jumpCooldown]]/1.35</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -373,17 +376,17 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="TabAbdomenParts" displayName="TabAbdomenParts" ref="A1:K10" totalsRowShown="0" headerRowDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="TabAbdomenParts" displayName="TabAbdomenParts" ref="A1:K10" totalsRowShown="0" headerRowDxfId="9">
   <autoFilter ref="A1:K10"/>
   <tableColumns count="11">
     <tableColumn id="1" name="ID"/>
-    <tableColumn id="2" name="name" dataDxfId="6">
+    <tableColumn id="2" name="name" dataDxfId="8">
       <calculatedColumnFormula>CONCATENATE("Beetle Abdomen ",A2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="description">
       <calculatedColumnFormula>CONCATENATE("A ", B2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="assetName" dataDxfId="5">
+    <tableColumn id="4" name="assetName" dataDxfId="7">
       <calculatedColumnFormula>CONCATENATE("beetle",A2,"-abdomen")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" name="health"/>
@@ -392,8 +395,8 @@
     <tableColumn id="8" name="jumpForce"/>
     <tableColumn id="9" name="backSpeed"/>
     <tableColumn id="10" name="jumpCooldown"/>
-    <tableColumn id="11" name="VALUE" dataDxfId="4">
-      <calculatedColumnFormula>TabAbdomenParts[[#This Row],[health]]/4+TabAbdomenParts[[#This Row],[damage]]/2+TabAbdomenParts[[#This Row],[turnSpeed]]+TabAbdomenParts[[#This Row],[jumpForce]]/200+TabAbdomenParts[[#This Row],[backSpeed]]/30</calculatedColumnFormula>
+    <tableColumn id="11" name="VALUE" dataDxfId="1">
+      <calculatedColumnFormula>TabAbdomenParts[[#This Row],[health]]/50+TabAbdomenParts[[#This Row],[damage]]/25+TabAbdomenParts[[#This Row],[turnSpeed]]/160+TabAbdomenParts[[#This Row],[jumpForce]]/1300+TabAbdomenParts[[#This Row],[backSpeed]]/25</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -401,17 +404,17 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="TabLegParts" displayName="TabLegParts" ref="A1:K6" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="TabLegParts" displayName="TabLegParts" ref="A1:K6" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="A1:K6"/>
   <tableColumns count="11">
     <tableColumn id="1" name="ID"/>
-    <tableColumn id="2" name="name" dataDxfId="2">
+    <tableColumn id="2" name="name" dataDxfId="5">
       <calculatedColumnFormula>CONCATENATE("Beetle Leg ",A2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="description">
       <calculatedColumnFormula>CONCATENATE("A ", B2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="assetName" dataDxfId="1">
+    <tableColumn id="4" name="assetName" dataDxfId="4">
       <calculatedColumnFormula>CONCATENATE("beetle",A2,)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" name="health"/>
@@ -421,7 +424,7 @@
     <tableColumn id="9" name="backSpeed"/>
     <tableColumn id="10" name="jumpCooldown"/>
     <tableColumn id="11" name="VALUE" dataDxfId="0">
-      <calculatedColumnFormula>TabLegParts[[#This Row],[health]]/4+TabLegParts[[#This Row],[damage]]/2+TabLegParts[[#This Row],[turnSpeed]]/60+TabLegParts[[#This Row],[jumpForce]]/200+TabLegParts[[#This Row],[backSpeed]]/60</calculatedColumnFormula>
+      <calculatedColumnFormula>TabLegParts[[#This Row],[health]]/50+TabLegParts[[#This Row],[damage]]/25+TabLegParts[[#This Row],[turnSpeed]]/160+TabLegParts[[#This Row],[jumpForce]]/1300+TabLegParts[[#This Row],[backSpeed]]/25</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -504,23 +507,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -556,23 +542,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -751,7 +720,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -809,67 +778,67 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B2" t="str">
         <f>CONCATENATE("Beetle Head ",A2)</f>
-        <v>Beetle Head 1</v>
+        <v>Beetle Head 8</v>
       </c>
       <c r="C2" t="str">
         <f>CONCATENATE("A ", B2)</f>
-        <v>A Beetle Head 1</v>
+        <v>A Beetle Head 8</v>
       </c>
       <c r="D2" t="str">
         <f>CONCATENATE("beetle",A2,"-head")</f>
-        <v>beetle1-head</v>
+        <v>beetle8-head</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="G2">
-        <v>60</v>
+        <v>-60</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="4">
         <v>0</v>
       </c>
       <c r="J2">
         <v>0</v>
       </c>
       <c r="K2">
-        <f>TabHeadParts[[#This Row],[health]]/4+TabHeadParts[[#This Row],[damage]]/4+TabHeadParts[[#This Row],[turnSpeed]]/60+TabHeadParts[[#This Row],[jumpForce]]/100+TabHeadParts[[#This Row],[backSpeed]]</f>
-        <v>3</v>
+        <f>TabHeadParts[[#This Row],[health]]/50+TabHeadParts[[#This Row],[damage]]/25+TabHeadParts[[#This Row],[turnSpeed]]/160+TabHeadParts[[#This Row],[jumpForce]]/1300+TabHeadParts[[#This Row],[backSpeed]]/25</f>
+        <v>0.82499999999999996</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" t="str">
-        <f t="shared" ref="B3:B5" si="0">CONCATENATE("Beetle Head ",A3)</f>
-        <v>Beetle Head 2</v>
+        <f>CONCATENATE("Beetle Head ",A3)</f>
+        <v>Beetle Head 4</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C5" si="1">CONCATENATE("A ", B3)</f>
-        <v>A Beetle Head 2</v>
+        <f>CONCATENATE("A ", B3)</f>
+        <v>A Beetle Head 4</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D5" si="2">CONCATENATE("beetle",A3,"-head")</f>
-        <v>beetle2-head</v>
+        <f>CONCATENATE("beetle",A3,"-head")</f>
+        <v>beetle4-head</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="G3">
-        <v>80</v>
+        <v>-28</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -881,8 +850,8 @@
         <v>0</v>
       </c>
       <c r="K3">
-        <f>TabHeadParts[[#This Row],[health]]/4+TabHeadParts[[#This Row],[damage]]/4+TabHeadParts[[#This Row],[turnSpeed]]/60+TabHeadParts[[#This Row],[jumpForce]]/100+TabHeadParts[[#This Row],[backSpeed]]</f>
-        <v>3.333333333333333</v>
+        <f>TabHeadParts[[#This Row],[health]]/50+TabHeadParts[[#This Row],[damage]]/25+TabHeadParts[[#This Row],[turnSpeed]]/160+TabHeadParts[[#This Row],[jumpForce]]/1300+TabHeadParts[[#This Row],[backSpeed]]/25</f>
+        <v>0.82499999999999996</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -890,25 +859,25 @@
         <v>3</v>
       </c>
       <c r="B4" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("Beetle Head ",A4)</f>
         <v>Beetle Head 3</v>
       </c>
       <c r="C4" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("A ", B4)</f>
         <v>A Beetle Head 3</v>
       </c>
       <c r="D4" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("beetle",A4,"-head")</f>
         <v>beetle3-head</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G4">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -920,34 +889,34 @@
         <v>0</v>
       </c>
       <c r="K4">
-        <f>TabHeadParts[[#This Row],[health]]/4+TabHeadParts[[#This Row],[damage]]/4+TabHeadParts[[#This Row],[turnSpeed]]/60+TabHeadParts[[#This Row],[jumpForce]]/100+TabHeadParts[[#This Row],[backSpeed]]</f>
-        <v>5.166666666666667</v>
+        <f>TabHeadParts[[#This Row],[health]]/50+TabHeadParts[[#This Row],[damage]]/25+TabHeadParts[[#This Row],[turnSpeed]]/160+TabHeadParts[[#This Row],[jumpForce]]/1300+TabHeadParts[[#This Row],[backSpeed]]/25</f>
+        <v>0.82500000000000007</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" t="str">
-        <f t="shared" si="0"/>
-        <v>Beetle Head 4</v>
+        <f>CONCATENATE("Beetle Head ",A5)</f>
+        <v>Beetle Head 2</v>
       </c>
       <c r="C5" t="str">
-        <f t="shared" si="1"/>
-        <v>A Beetle Head 4</v>
+        <f>CONCATENATE("A ", B5)</f>
+        <v>A Beetle Head 2</v>
       </c>
       <c r="D5" t="str">
-        <f t="shared" si="2"/>
-        <v>beetle4-head</v>
+        <f>CONCATENATE("beetle",A5,"-head")</f>
+        <v>beetle2-head</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -959,8 +928,8 @@
         <v>0</v>
       </c>
       <c r="K5">
-        <f>TabHeadParts[[#This Row],[health]]/4+TabHeadParts[[#This Row],[damage]]/4+TabHeadParts[[#This Row],[turnSpeed]]/60+TabHeadParts[[#This Row],[jumpForce]]/100+TabHeadParts[[#This Row],[backSpeed]]</f>
-        <v>5</v>
+        <f>TabHeadParts[[#This Row],[health]]/50+TabHeadParts[[#This Row],[damage]]/25+TabHeadParts[[#This Row],[turnSpeed]]/160+TabHeadParts[[#This Row],[jumpForce]]/1300+TabHeadParts[[#This Row],[backSpeed]]/25</f>
+        <v>0.82499999999999996</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -983,10 +952,10 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G6">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -998,8 +967,8 @@
         <v>0</v>
       </c>
       <c r="K6">
-        <f>TabHeadParts[[#This Row],[health]]/4+TabHeadParts[[#This Row],[damage]]/4+TabHeadParts[[#This Row],[turnSpeed]]/60+TabHeadParts[[#This Row],[jumpForce]]/100+TabHeadParts[[#This Row],[backSpeed]]</f>
-        <v>2.3333333333333335</v>
+        <f>TabHeadParts[[#This Row],[health]]/50+TabHeadParts[[#This Row],[damage]]/25+TabHeadParts[[#This Row],[turnSpeed]]/160+TabHeadParts[[#This Row],[jumpForce]]/1300+TabHeadParts[[#This Row],[backSpeed]]/25</f>
+        <v>0.83</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1022,10 +991,10 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G7">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -1037,73 +1006,73 @@
         <v>0</v>
       </c>
       <c r="K7">
-        <f>TabHeadParts[[#This Row],[health]]/4+TabHeadParts[[#This Row],[damage]]/4+TabHeadParts[[#This Row],[turnSpeed]]/60+TabHeadParts[[#This Row],[jumpForce]]/100+TabHeadParts[[#This Row],[backSpeed]]</f>
-        <v>2.6666666666666665</v>
+        <f>TabHeadParts[[#This Row],[health]]/50+TabHeadParts[[#This Row],[damage]]/25+TabHeadParts[[#This Row],[turnSpeed]]/160+TabHeadParts[[#This Row],[jumpForce]]/1300+TabHeadParts[[#This Row],[backSpeed]]/25</f>
+        <v>0.82499999999999996</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B8" t="str">
         <f>CONCATENATE("Beetle Head ",A8)</f>
-        <v>Beetle Head 7</v>
+        <v>Beetle Head 1</v>
       </c>
       <c r="C8" t="str">
         <f>CONCATENATE("A ", B8)</f>
-        <v>A Beetle Head 7</v>
+        <v>A Beetle Head 1</v>
       </c>
       <c r="D8" t="str">
         <f>CONCATENATE("beetle",A8,"-head")</f>
-        <v>beetle7-head</v>
+        <v>beetle1-head</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G8">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8">
         <v>0</v>
       </c>
       <c r="J8">
         <v>0</v>
       </c>
       <c r="K8">
-        <f>TabHeadParts[[#This Row],[health]]/4+TabHeadParts[[#This Row],[damage]]/4+TabHeadParts[[#This Row],[turnSpeed]]/60+TabHeadParts[[#This Row],[jumpForce]]/100+TabHeadParts[[#This Row],[backSpeed]]</f>
-        <v>3.3333333333333335</v>
+        <f>TabHeadParts[[#This Row],[health]]/50+TabHeadParts[[#This Row],[damage]]/25+TabHeadParts[[#This Row],[turnSpeed]]/160+TabHeadParts[[#This Row],[jumpForce]]/1300+TabHeadParts[[#This Row],[backSpeed]]/25</f>
+        <v>0.82000000000000006</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" t="str">
         <f>CONCATENATE("Beetle Head ",A9)</f>
-        <v>Beetle Head 8</v>
+        <v>Beetle Head 9</v>
       </c>
       <c r="C9" t="str">
         <f>CONCATENATE("A ", B9)</f>
-        <v>A Beetle Head 8</v>
+        <v>A Beetle Head 9</v>
       </c>
       <c r="D9" t="str">
         <f>CONCATENATE("beetle",A9,"-head")</f>
-        <v>beetle8-head</v>
+        <v>beetle9-head</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -1115,34 +1084,34 @@
         <v>0</v>
       </c>
       <c r="K9">
-        <f>TabHeadParts[[#This Row],[health]]/4+TabHeadParts[[#This Row],[damage]]/4+TabHeadParts[[#This Row],[turnSpeed]]/60+TabHeadParts[[#This Row],[jumpForce]]/100+TabHeadParts[[#This Row],[backSpeed]]</f>
-        <v>6</v>
+        <f>TabHeadParts[[#This Row],[health]]/50+TabHeadParts[[#This Row],[damage]]/25+TabHeadParts[[#This Row],[turnSpeed]]/160+TabHeadParts[[#This Row],[jumpForce]]/1300+TabHeadParts[[#This Row],[backSpeed]]/25</f>
+        <v>0.82499999999999996</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B10" t="str">
         <f>CONCATENATE("Beetle Head ",A10)</f>
-        <v>Beetle Head 9</v>
+        <v>Beetle Head 7</v>
       </c>
       <c r="C10" t="str">
         <f>CONCATENATE("A ", B10)</f>
-        <v>A Beetle Head 9</v>
+        <v>A Beetle Head 7</v>
       </c>
       <c r="D10" t="str">
         <f>CONCATENATE("beetle",A10,"-head")</f>
-        <v>beetle9-head</v>
+        <v>beetle7-head</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="G10">
-        <v>40</v>
+        <v>112</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -1154,8 +1123,8 @@
         <v>0</v>
       </c>
       <c r="K10">
-        <f>TabHeadParts[[#This Row],[health]]/4+TabHeadParts[[#This Row],[damage]]/4+TabHeadParts[[#This Row],[turnSpeed]]/60+TabHeadParts[[#This Row],[jumpForce]]/100+TabHeadParts[[#This Row],[backSpeed]]</f>
-        <v>3.6666666666666665</v>
+        <f>TabHeadParts[[#This Row],[health]]/50+TabHeadParts[[#This Row],[damage]]/25+TabHeadParts[[#This Row],[turnSpeed]]/160+TabHeadParts[[#This Row],[jumpForce]]/1300+TabHeadParts[[#This Row],[backSpeed]]/25</f>
+        <v>0.82</v>
       </c>
     </row>
   </sheetData>
@@ -1172,7 +1141,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1241,26 +1210,26 @@
         <v>beetle1-thorax</v>
       </c>
       <c r="E2">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2">
-        <v>1300</v>
+        <v>1400</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2">
-        <v>1.7</v>
+        <v>0.95</v>
       </c>
       <c r="K2">
-        <f>TabThoraxParts[[#This Row],[health]]/4+TabThoraxParts[[#This Row],[damage]]/2+TabThoraxParts[[#This Row],[turnSpeed]]+TabThoraxParts[[#This Row],[jumpForce]]/200+TabThoraxParts[[#This Row],[backSpeed]]</f>
-        <v>8.5</v>
+        <f>TabThoraxParts[[#This Row],[health]]/50+TabThoraxParts[[#This Row],[damage]]/25+TabThoraxParts[[#This Row],[turnSpeed]]/160+TabThoraxParts[[#This Row],[jumpForce]]/1300+TabThoraxParts[[#This Row],[backSpeed]]/25+1/TabThoraxParts[[#This Row],[jumpCooldown]]/1.35</f>
+        <v>2.3366501724396462</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1280,13 +1249,13 @@
         <v>beetle2-thorax</v>
       </c>
       <c r="E3">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="H3">
         <v>700</v>
@@ -1295,11 +1264,11 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="K3">
-        <f>TabThoraxParts[[#This Row],[health]]/4+TabThoraxParts[[#This Row],[damage]]/2+TabThoraxParts[[#This Row],[turnSpeed]]+TabThoraxParts[[#This Row],[jumpForce]]/200+TabThoraxParts[[#This Row],[backSpeed]]</f>
-        <v>6.5</v>
+        <f>TabThoraxParts[[#This Row],[health]]/50+TabThoraxParts[[#This Row],[damage]]/25+TabThoraxParts[[#This Row],[turnSpeed]]/160+TabThoraxParts[[#This Row],[jumpForce]]/1300+TabThoraxParts[[#This Row],[backSpeed]]/25+1/TabThoraxParts[[#This Row],[jumpCooldown]]/1.35</f>
+        <v>2.32781339031339</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1319,26 +1288,26 @@
         <v>beetle3-thorax</v>
       </c>
       <c r="E4">
-        <v>10</v>
+        <v>-14</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4">
-        <v>800</v>
+        <v>1500</v>
       </c>
       <c r="I4">
         <v>0</v>
       </c>
       <c r="J4">
-        <v>0.9</v>
+        <v>0.4</v>
       </c>
       <c r="K4">
-        <f>TabThoraxParts[[#This Row],[health]]/4+TabThoraxParts[[#This Row],[damage]]/2+TabThoraxParts[[#This Row],[turnSpeed]]+TabThoraxParts[[#This Row],[jumpForce]]/200+TabThoraxParts[[#This Row],[backSpeed]]</f>
-        <v>6.5</v>
+        <f>TabThoraxParts[[#This Row],[health]]/50+TabThoraxParts[[#This Row],[damage]]/25+TabThoraxParts[[#This Row],[turnSpeed]]/160+TabThoraxParts[[#This Row],[jumpForce]]/1300+TabThoraxParts[[#This Row],[backSpeed]]/25+1/TabThoraxParts[[#This Row],[jumpCooldown]]/1.35</f>
+        <v>2.3256980056980052</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1358,26 +1327,26 @@
         <v>beetle4-thorax</v>
       </c>
       <c r="E5">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="H5">
-        <v>1100</v>
+        <v>900</v>
       </c>
       <c r="I5">
         <v>0</v>
       </c>
       <c r="J5">
-        <v>1.3</v>
+        <v>0.8</v>
       </c>
       <c r="K5">
-        <f>TabThoraxParts[[#This Row],[health]]/4+TabThoraxParts[[#This Row],[damage]]/2+TabThoraxParts[[#This Row],[turnSpeed]]+TabThoraxParts[[#This Row],[jumpForce]]/200+TabThoraxParts[[#This Row],[backSpeed]]</f>
-        <v>7.5</v>
+        <f>TabThoraxParts[[#This Row],[health]]/50+TabThoraxParts[[#This Row],[damage]]/25+TabThoraxParts[[#This Row],[turnSpeed]]/160+TabThoraxParts[[#This Row],[jumpForce]]/1300+TabThoraxParts[[#This Row],[backSpeed]]/25+1/TabThoraxParts[[#This Row],[jumpCooldown]]/1.35</f>
+        <v>2.3307336182336185</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1397,26 +1366,26 @@
         <v>beetle5-thorax</v>
       </c>
       <c r="E6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6">
-        <v>1500</v>
+        <v>1800</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6">
-        <v>1.8</v>
+        <v>1</v>
       </c>
       <c r="K6">
-        <f>TabThoraxParts[[#This Row],[health]]/4+TabThoraxParts[[#This Row],[damage]]/2+TabThoraxParts[[#This Row],[turnSpeed]]+TabThoraxParts[[#This Row],[jumpForce]]/200+TabThoraxParts[[#This Row],[backSpeed]]</f>
-        <v>8.5</v>
+        <f>TabThoraxParts[[#This Row],[health]]/50+TabThoraxParts[[#This Row],[damage]]/25+TabThoraxParts[[#This Row],[turnSpeed]]/160+TabThoraxParts[[#This Row],[jumpForce]]/1300+TabThoraxParts[[#This Row],[backSpeed]]/25+1/TabThoraxParts[[#This Row],[jumpCooldown]]/1.35</f>
+        <v>2.3253561253561252</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1436,26 +1405,26 @@
         <v>beetle6-thorax</v>
       </c>
       <c r="E7">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7">
-        <v>1100</v>
+        <v>1000</v>
       </c>
       <c r="I7">
         <v>0</v>
       </c>
       <c r="J7">
-        <v>1.3</v>
+        <v>0.6</v>
       </c>
       <c r="K7">
-        <f>TabThoraxParts[[#This Row],[health]]/4+TabThoraxParts[[#This Row],[damage]]/2+TabThoraxParts[[#This Row],[turnSpeed]]+TabThoraxParts[[#This Row],[jumpForce]]/200+TabThoraxParts[[#This Row],[backSpeed]]</f>
-        <v>8.5</v>
+        <f>TabThoraxParts[[#This Row],[health]]/50+TabThoraxParts[[#This Row],[damage]]/25+TabThoraxParts[[#This Row],[turnSpeed]]/160+TabThoraxParts[[#This Row],[jumpForce]]/1300+TabThoraxParts[[#This Row],[backSpeed]]/25+1/TabThoraxParts[[#This Row],[jumpCooldown]]/1.35</f>
+        <v>2.3237986704653371</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1475,26 +1444,26 @@
         <v>beetle7-thorax</v>
       </c>
       <c r="E8">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8">
-        <v>1100</v>
+        <v>2000</v>
       </c>
       <c r="I8">
         <v>0</v>
       </c>
       <c r="J8">
-        <v>1.3</v>
+        <v>0.75</v>
       </c>
       <c r="K8">
-        <f>TabThoraxParts[[#This Row],[health]]/4+TabThoraxParts[[#This Row],[damage]]/2+TabThoraxParts[[#This Row],[turnSpeed]]+TabThoraxParts[[#This Row],[jumpForce]]/200+TabThoraxParts[[#This Row],[backSpeed]]</f>
-        <v>8</v>
+        <f>TabThoraxParts[[#This Row],[health]]/50+TabThoraxParts[[#This Row],[damage]]/25+TabThoraxParts[[#This Row],[turnSpeed]]/160+TabThoraxParts[[#This Row],[jumpForce]]/1300+TabThoraxParts[[#This Row],[backSpeed]]/25+1/TabThoraxParts[[#This Row],[jumpCooldown]]/1.35</f>
+        <v>2.3261158594491929</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1514,26 +1483,26 @@
         <v>beetle8-thorax</v>
       </c>
       <c r="E9">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="H9">
-        <v>900</v>
+        <v>800</v>
       </c>
       <c r="I9">
         <v>0</v>
       </c>
       <c r="J9">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="K9">
-        <f>TabThoraxParts[[#This Row],[health]]/4+TabThoraxParts[[#This Row],[damage]]/2+TabThoraxParts[[#This Row],[turnSpeed]]+TabThoraxParts[[#This Row],[jumpForce]]/200+TabThoraxParts[[#This Row],[backSpeed]]</f>
-        <v>6.5</v>
+        <f>TabThoraxParts[[#This Row],[health]]/50+TabThoraxParts[[#This Row],[damage]]/25+TabThoraxParts[[#This Row],[turnSpeed]]/160+TabThoraxParts[[#This Row],[jumpForce]]/1300+TabThoraxParts[[#This Row],[backSpeed]]/25+1/TabThoraxParts[[#This Row],[jumpCooldown]]/1.35</f>
+        <v>2.3098356735856735</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1553,10 +1522,10 @@
         <v>beetle9-thorax</v>
       </c>
       <c r="E10">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -1568,14 +1537,26 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="K10">
-        <f>TabThoraxParts[[#This Row],[health]]/4+TabThoraxParts[[#This Row],[damage]]/2+TabThoraxParts[[#This Row],[turnSpeed]]+TabThoraxParts[[#This Row],[jumpForce]]/200+TabThoraxParts[[#This Row],[backSpeed]]</f>
-        <v>7.5</v>
+        <f>TabThoraxParts[[#This Row],[health]]/50+TabThoraxParts[[#This Row],[damage]]/25+TabThoraxParts[[#This Row],[turnSpeed]]/160+TabThoraxParts[[#This Row],[jumpForce]]/1300+TabThoraxParts[[#This Row],[backSpeed]]/25+1/TabThoraxParts[[#This Row],[jumpCooldown]]/1.35</f>
+        <v>2.3290028490028489</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="K2:K10">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -1588,7 +1569,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I10"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1657,7 +1638,7 @@
         <v>beetle1-abdomen</v>
       </c>
       <c r="E2">
-        <v>36</v>
+        <v>75</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -1669,14 +1650,14 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J2">
         <v>0</v>
       </c>
       <c r="K2">
-        <f>TabAbdomenParts[[#This Row],[health]]/4+TabAbdomenParts[[#This Row],[damage]]/2+TabAbdomenParts[[#This Row],[turnSpeed]]+TabAbdomenParts[[#This Row],[jumpForce]]/200+TabAbdomenParts[[#This Row],[backSpeed]]/30</f>
-        <v>9.1</v>
+        <f>TabAbdomenParts[[#This Row],[health]]/50+TabAbdomenParts[[#This Row],[damage]]/25+TabAbdomenParts[[#This Row],[turnSpeed]]/160+TabAbdomenParts[[#This Row],[jumpForce]]/1300+TabAbdomenParts[[#This Row],[backSpeed]]/25</f>
+        <v>1.7</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1696,7 +1677,7 @@
         <v>beetle2-abdomen</v>
       </c>
       <c r="E3">
-        <v>34</v>
+        <v>70</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1708,14 +1689,14 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J3">
         <v>0</v>
       </c>
       <c r="K3">
-        <f>TabAbdomenParts[[#This Row],[health]]/4+TabAbdomenParts[[#This Row],[damage]]/2+TabAbdomenParts[[#This Row],[turnSpeed]]+TabAbdomenParts[[#This Row],[jumpForce]]/200+TabAbdomenParts[[#This Row],[backSpeed]]/30</f>
-        <v>8.5666666666666664</v>
+        <f>TabAbdomenParts[[#This Row],[health]]/50+TabAbdomenParts[[#This Row],[damage]]/25+TabAbdomenParts[[#This Row],[turnSpeed]]/160+TabAbdomenParts[[#This Row],[jumpForce]]/1300+TabAbdomenParts[[#This Row],[backSpeed]]/25</f>
+        <v>1.72</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1735,7 +1716,7 @@
         <v>beetle3-abdomen</v>
       </c>
       <c r="E4">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -1747,14 +1728,14 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="J4">
         <v>0</v>
       </c>
       <c r="K4">
-        <f>TabAbdomenParts[[#This Row],[health]]/4+TabAbdomenParts[[#This Row],[damage]]/2+TabAbdomenParts[[#This Row],[turnSpeed]]+TabAbdomenParts[[#This Row],[jumpForce]]/200+TabAbdomenParts[[#This Row],[backSpeed]]/30</f>
-        <v>7.2</v>
+        <f>TabAbdomenParts[[#This Row],[health]]/50+TabAbdomenParts[[#This Row],[damage]]/25+TabAbdomenParts[[#This Row],[turnSpeed]]/160+TabAbdomenParts[[#This Row],[jumpForce]]/1300+TabAbdomenParts[[#This Row],[backSpeed]]/25</f>
+        <v>1.7</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1774,7 +1755,7 @@
         <v>beetle4-abdomen</v>
       </c>
       <c r="E5">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -1786,14 +1767,14 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="J5">
         <v>0</v>
       </c>
       <c r="K5">
-        <f>TabAbdomenParts[[#This Row],[health]]/4+TabAbdomenParts[[#This Row],[damage]]/2+TabAbdomenParts[[#This Row],[turnSpeed]]+TabAbdomenParts[[#This Row],[jumpForce]]/200+TabAbdomenParts[[#This Row],[backSpeed]]/30</f>
-        <v>7.5666666666666664</v>
+        <f>TabAbdomenParts[[#This Row],[health]]/50+TabAbdomenParts[[#This Row],[damage]]/25+TabAbdomenParts[[#This Row],[turnSpeed]]/160+TabAbdomenParts[[#This Row],[jumpForce]]/1300+TabAbdomenParts[[#This Row],[backSpeed]]/25</f>
+        <v>1.72</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1813,7 +1794,7 @@
         <v>beetle5-abdomen</v>
       </c>
       <c r="E6">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -1825,14 +1806,14 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="J6">
         <v>0</v>
       </c>
       <c r="K6">
-        <f>TabAbdomenParts[[#This Row],[health]]/4+TabAbdomenParts[[#This Row],[damage]]/2+TabAbdomenParts[[#This Row],[turnSpeed]]+TabAbdomenParts[[#This Row],[jumpForce]]/200+TabAbdomenParts[[#This Row],[backSpeed]]/30</f>
-        <v>6.5333333333333332</v>
+        <f>TabAbdomenParts[[#This Row],[health]]/50+TabAbdomenParts[[#This Row],[damage]]/25+TabAbdomenParts[[#This Row],[turnSpeed]]/160+TabAbdomenParts[[#This Row],[jumpForce]]/1300+TabAbdomenParts[[#This Row],[backSpeed]]/25</f>
+        <v>1.7</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1852,7 +1833,7 @@
         <v>beetle6-abdomen</v>
       </c>
       <c r="E7">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -1864,14 +1845,14 @@
         <v>0</v>
       </c>
       <c r="I7">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="J7">
         <v>0</v>
       </c>
       <c r="K7">
-        <f>TabAbdomenParts[[#This Row],[health]]/4+TabAbdomenParts[[#This Row],[damage]]/2+TabAbdomenParts[[#This Row],[turnSpeed]]+TabAbdomenParts[[#This Row],[jumpForce]]/200+TabAbdomenParts[[#This Row],[backSpeed]]/30</f>
-        <v>7.6333333333333337</v>
+        <f>TabAbdomenParts[[#This Row],[health]]/50+TabAbdomenParts[[#This Row],[damage]]/25+TabAbdomenParts[[#This Row],[turnSpeed]]/160+TabAbdomenParts[[#This Row],[jumpForce]]/1300+TabAbdomenParts[[#This Row],[backSpeed]]/25</f>
+        <v>1.7000000000000002</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1891,7 +1872,7 @@
         <v>beetle7-abdomen</v>
       </c>
       <c r="E8">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -1903,14 +1884,14 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="J8">
         <v>0</v>
       </c>
       <c r="K8">
-        <f>TabAbdomenParts[[#This Row],[health]]/4+TabAbdomenParts[[#This Row],[damage]]/2+TabAbdomenParts[[#This Row],[turnSpeed]]+TabAbdomenParts[[#This Row],[jumpForce]]/200+TabAbdomenParts[[#This Row],[backSpeed]]/30</f>
-        <v>8.1999999999999993</v>
+        <f>TabAbdomenParts[[#This Row],[health]]/50+TabAbdomenParts[[#This Row],[damage]]/25+TabAbdomenParts[[#This Row],[turnSpeed]]/160+TabAbdomenParts[[#This Row],[jumpForce]]/1300+TabAbdomenParts[[#This Row],[backSpeed]]/25</f>
+        <v>1.7000000000000002</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1930,7 +1911,7 @@
         <v>beetle8-abdomen</v>
       </c>
       <c r="E9">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -1942,14 +1923,14 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="J9">
         <v>0</v>
       </c>
       <c r="K9">
-        <f>TabAbdomenParts[[#This Row],[health]]/4+TabAbdomenParts[[#This Row],[damage]]/2+TabAbdomenParts[[#This Row],[turnSpeed]]+TabAbdomenParts[[#This Row],[jumpForce]]/200+TabAbdomenParts[[#This Row],[backSpeed]]/30</f>
-        <v>7.1</v>
+        <f>TabAbdomenParts[[#This Row],[health]]/50+TabAbdomenParts[[#This Row],[damage]]/25+TabAbdomenParts[[#This Row],[turnSpeed]]/160+TabAbdomenParts[[#This Row],[jumpForce]]/1300+TabAbdomenParts[[#This Row],[backSpeed]]/25</f>
+        <v>1.7200000000000002</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1969,7 +1950,7 @@
         <v>beetle9-abdomen</v>
       </c>
       <c r="E10">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -1981,17 +1962,29 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="J10">
         <v>0</v>
       </c>
       <c r="K10">
-        <f>TabAbdomenParts[[#This Row],[health]]/4+TabAbdomenParts[[#This Row],[damage]]/2+TabAbdomenParts[[#This Row],[turnSpeed]]+TabAbdomenParts[[#This Row],[jumpForce]]/200+TabAbdomenParts[[#This Row],[backSpeed]]/30</f>
-        <v>7.5666666666666664</v>
+        <f>TabAbdomenParts[[#This Row],[health]]/50+TabAbdomenParts[[#This Row],[damage]]/25+TabAbdomenParts[[#This Row],[turnSpeed]]/160+TabAbdomenParts[[#This Row],[jumpForce]]/1300+TabAbdomenParts[[#This Row],[backSpeed]]/25</f>
+        <v>1.72</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="K2:K10">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
@@ -2004,8 +1997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2080,20 +2073,20 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="J2">
         <v>0</v>
       </c>
       <c r="K2" s="2">
-        <f>TabLegParts[[#This Row],[health]]/4+TabLegParts[[#This Row],[damage]]/2+TabLegParts[[#This Row],[turnSpeed]]/60+TabLegParts[[#This Row],[jumpForce]]/200+TabLegParts[[#This Row],[backSpeed]]/60</f>
-        <v>2.1333333333333333</v>
+        <f>TabLegParts[[#This Row],[health]]/50+TabLegParts[[#This Row],[damage]]/25+TabLegParts[[#This Row],[turnSpeed]]/160+TabLegParts[[#This Row],[jumpForce]]/1300+TabLegParts[[#This Row],[backSpeed]]/25</f>
+        <v>0.995</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -2119,20 +2112,20 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J3">
         <v>0</v>
       </c>
       <c r="K3" s="3">
-        <f>TabLegParts[[#This Row],[health]]/4+TabLegParts[[#This Row],[damage]]/2+TabLegParts[[#This Row],[turnSpeed]]/60+TabLegParts[[#This Row],[jumpForce]]/200+TabLegParts[[#This Row],[backSpeed]]/60</f>
-        <v>1.3333333333333335</v>
+        <f>TabLegParts[[#This Row],[health]]/50+TabLegParts[[#This Row],[damage]]/25+TabLegParts[[#This Row],[turnSpeed]]/160+TabLegParts[[#This Row],[jumpForce]]/1300+TabLegParts[[#This Row],[backSpeed]]/25</f>
+        <v>0.97499999999999998</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -2158,20 +2151,20 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="J4">
         <v>0</v>
       </c>
       <c r="K4" s="2">
-        <f>TabLegParts[[#This Row],[health]]/4+TabLegParts[[#This Row],[damage]]/2+TabLegParts[[#This Row],[turnSpeed]]/60+TabLegParts[[#This Row],[jumpForce]]/200+TabLegParts[[#This Row],[backSpeed]]/60</f>
-        <v>1.4</v>
+        <f>TabLegParts[[#This Row],[health]]/50+TabLegParts[[#This Row],[damage]]/25+TabLegParts[[#This Row],[turnSpeed]]/160+TabLegParts[[#This Row],[jumpForce]]/1300+TabLegParts[[#This Row],[backSpeed]]/25</f>
+        <v>0.98499999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -2197,20 +2190,20 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="J5">
         <v>0</v>
       </c>
       <c r="K5" s="3">
-        <f>TabLegParts[[#This Row],[health]]/4+TabLegParts[[#This Row],[damage]]/2+TabLegParts[[#This Row],[turnSpeed]]/60+TabLegParts[[#This Row],[jumpForce]]/200+TabLegParts[[#This Row],[backSpeed]]/60</f>
-        <v>1.8666666666666667</v>
+        <f>TabLegParts[[#This Row],[health]]/50+TabLegParts[[#This Row],[damage]]/25+TabLegParts[[#This Row],[turnSpeed]]/160+TabLegParts[[#This Row],[jumpForce]]/1300+TabLegParts[[#This Row],[backSpeed]]/25</f>
+        <v>0.99</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -2236,23 +2229,35 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J6">
         <v>0</v>
       </c>
       <c r="K6" s="2">
-        <f>TabLegParts[[#This Row],[health]]/4+TabLegParts[[#This Row],[damage]]/2+TabLegParts[[#This Row],[turnSpeed]]/60+TabLegParts[[#This Row],[jumpForce]]/200+TabLegParts[[#This Row],[backSpeed]]/60</f>
-        <v>1.2666666666666666</v>
+        <f>TabLegParts[[#This Row],[health]]/50+TabLegParts[[#This Row],[damage]]/25+TabLegParts[[#This Row],[turnSpeed]]/160+TabLegParts[[#This Row],[jumpForce]]/1300+TabLegParts[[#This Row],[backSpeed]]/25</f>
+        <v>0.97</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="K2:K6">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
new data values up to beetle 14
</commit_message>
<xml_diff>
--- a/UnityProject/LD35/Assets/StaticDefinitions/BodyPartDefs.xlsx
+++ b/UnityProject/LD35/Assets/StaticDefinitions/BodyPartDefs.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LD35\trunk\UnityProject\LD35\Assets\StaticDefinitions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UnityProjects\ld35-master\UnityProject\LD35\Assets\StaticDefinitions\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="3120" windowWidth="22035" windowHeight="9285"/>
+    <workbookView xWindow="120" yWindow="3120" windowWidth="22035" windowHeight="9285" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="HeadPartDefs" sheetId="5" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="AbdomenPartDefs" sheetId="3" r:id="rId3"/>
     <sheet name="LegPartDefs" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -317,8 +317,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TabHeadParts" displayName="TabHeadParts" ref="A1:K10" totalsRowShown="0" headerRowDxfId="14">
-  <autoFilter ref="A1:K10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TabHeadParts" displayName="TabHeadParts" ref="A1:K15" totalsRowShown="0" headerRowDxfId="14">
+  <autoFilter ref="A1:K15"/>
   <sortState ref="A2:K10">
     <sortCondition ref="A1:A10"/>
   </sortState>
@@ -348,8 +348,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TabThoraxParts" displayName="TabThoraxParts" ref="A1:K10" totalsRowShown="0" headerRowDxfId="11">
-  <autoFilter ref="A1:K10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TabThoraxParts" displayName="TabThoraxParts" ref="A1:K15" totalsRowShown="0" headerRowDxfId="11">
+  <autoFilter ref="A1:K15"/>
   <tableColumns count="11">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="name" dataDxfId="10">
@@ -376,8 +376,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="TabAbdomenParts" displayName="TabAbdomenParts" ref="A1:K10" totalsRowShown="0" headerRowDxfId="7">
-  <autoFilter ref="A1:K10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="TabAbdomenParts" displayName="TabAbdomenParts" ref="A1:K15" totalsRowShown="0" headerRowDxfId="7">
+  <autoFilter ref="A1:K15"/>
   <tableColumns count="11">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="name" dataDxfId="6">
@@ -507,6 +507,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -542,6 +559,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -718,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -781,15 +815,15 @@
         <v>1</v>
       </c>
       <c r="B2" t="str">
-        <f>CONCATENATE("Beetle Head ",A2)</f>
+        <f t="shared" ref="B2:B10" si="0">CONCATENATE("Beetle Head ",A2)</f>
         <v>Beetle Head 1</v>
       </c>
       <c r="C2" t="str">
-        <f>CONCATENATE("A ", B2)</f>
+        <f t="shared" ref="C2:C10" si="1">CONCATENATE("A ", B2)</f>
         <v>A Beetle Head 1</v>
       </c>
       <c r="D2" t="str">
-        <f>CONCATENATE("beetle",A2,"-head")</f>
+        <f t="shared" ref="D2:D10" si="2">CONCATENATE("beetle",A2,"-head")</f>
         <v>beetle1-head</v>
       </c>
       <c r="E2">
@@ -820,15 +854,15 @@
         <v>2</v>
       </c>
       <c r="B3" t="str">
-        <f>CONCATENATE("Beetle Head ",A3)</f>
+        <f t="shared" si="0"/>
         <v>Beetle Head 2</v>
       </c>
       <c r="C3" t="str">
-        <f>CONCATENATE("A ", B3)</f>
+        <f t="shared" si="1"/>
         <v>A Beetle Head 2</v>
       </c>
       <c r="D3" t="str">
-        <f>CONCATENATE("beetle",A3,"-head")</f>
+        <f t="shared" si="2"/>
         <v>beetle2-head</v>
       </c>
       <c r="E3">
@@ -859,15 +893,15 @@
         <v>3</v>
       </c>
       <c r="B4" t="str">
-        <f>CONCATENATE("Beetle Head ",A4)</f>
+        <f t="shared" si="0"/>
         <v>Beetle Head 3</v>
       </c>
       <c r="C4" t="str">
-        <f>CONCATENATE("A ", B4)</f>
+        <f t="shared" si="1"/>
         <v>A Beetle Head 3</v>
       </c>
       <c r="D4" t="str">
-        <f>CONCATENATE("beetle",A4,"-head")</f>
+        <f t="shared" si="2"/>
         <v>beetle3-head</v>
       </c>
       <c r="E4">
@@ -898,15 +932,15 @@
         <v>4</v>
       </c>
       <c r="B5" t="str">
-        <f>CONCATENATE("Beetle Head ",A5)</f>
+        <f t="shared" si="0"/>
         <v>Beetle Head 4</v>
       </c>
       <c r="C5" t="str">
-        <f>CONCATENATE("A ", B5)</f>
+        <f t="shared" si="1"/>
         <v>A Beetle Head 4</v>
       </c>
       <c r="D5" t="str">
-        <f>CONCATENATE("beetle",A5,"-head")</f>
+        <f t="shared" si="2"/>
         <v>beetle4-head</v>
       </c>
       <c r="E5">
@@ -937,15 +971,15 @@
         <v>5</v>
       </c>
       <c r="B6" t="str">
-        <f>CONCATENATE("Beetle Head ",A6)</f>
+        <f t="shared" si="0"/>
         <v>Beetle Head 5</v>
       </c>
       <c r="C6" t="str">
-        <f>CONCATENATE("A ", B6)</f>
+        <f t="shared" si="1"/>
         <v>A Beetle Head 5</v>
       </c>
       <c r="D6" t="str">
-        <f>CONCATENATE("beetle",A6,"-head")</f>
+        <f t="shared" si="2"/>
         <v>beetle5-head</v>
       </c>
       <c r="E6">
@@ -976,15 +1010,15 @@
         <v>6</v>
       </c>
       <c r="B7" t="str">
-        <f>CONCATENATE("Beetle Head ",A7)</f>
+        <f t="shared" si="0"/>
         <v>Beetle Head 6</v>
       </c>
       <c r="C7" t="str">
-        <f>CONCATENATE("A ", B7)</f>
+        <f t="shared" si="1"/>
         <v>A Beetle Head 6</v>
       </c>
       <c r="D7" t="str">
-        <f>CONCATENATE("beetle",A7,"-head")</f>
+        <f t="shared" si="2"/>
         <v>beetle6-head</v>
       </c>
       <c r="E7">
@@ -1015,15 +1049,15 @@
         <v>7</v>
       </c>
       <c r="B8" t="str">
-        <f>CONCATENATE("Beetle Head ",A8)</f>
+        <f t="shared" si="0"/>
         <v>Beetle Head 7</v>
       </c>
       <c r="C8" t="str">
-        <f>CONCATENATE("A ", B8)</f>
+        <f t="shared" si="1"/>
         <v>A Beetle Head 7</v>
       </c>
       <c r="D8" t="str">
-        <f>CONCATENATE("beetle",A8,"-head")</f>
+        <f t="shared" si="2"/>
         <v>beetle7-head</v>
       </c>
       <c r="E8">
@@ -1054,15 +1088,15 @@
         <v>8</v>
       </c>
       <c r="B9" t="str">
-        <f>CONCATENATE("Beetle Head ",A9)</f>
+        <f t="shared" si="0"/>
         <v>Beetle Head 8</v>
       </c>
       <c r="C9" t="str">
-        <f>CONCATENATE("A ", B9)</f>
+        <f t="shared" si="1"/>
         <v>A Beetle Head 8</v>
       </c>
       <c r="D9" t="str">
-        <f>CONCATENATE("beetle",A9,"-head")</f>
+        <f t="shared" si="2"/>
         <v>beetle8-head</v>
       </c>
       <c r="E9">
@@ -1093,15 +1127,15 @@
         <v>9</v>
       </c>
       <c r="B10" t="str">
-        <f>CONCATENATE("Beetle Head ",A10)</f>
+        <f t="shared" si="0"/>
         <v>Beetle Head 9</v>
       </c>
       <c r="C10" t="str">
-        <f>CONCATENATE("A ", B10)</f>
+        <f t="shared" si="1"/>
         <v>A Beetle Head 9</v>
       </c>
       <c r="D10" t="str">
-        <f>CONCATENATE("beetle",A10,"-head")</f>
+        <f t="shared" si="2"/>
         <v>beetle9-head</v>
       </c>
       <c r="E10">
@@ -1125,6 +1159,201 @@
       <c r="K10">
         <f>TabHeadParts[[#This Row],[health]]/50+TabHeadParts[[#This Row],[damage]]/25+TabHeadParts[[#This Row],[turnSpeed]]/160+TabHeadParts[[#This Row],[jumpForce]]/1300+TabHeadParts[[#This Row],[backSpeed]]/25</f>
         <v>0.82499999999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="str">
+        <f>CONCATENATE("Beetle Head ",A11)</f>
+        <v>Beetle Head 10</v>
+      </c>
+      <c r="C11" t="str">
+        <f>CONCATENATE("A ", B11)</f>
+        <v>A Beetle Head 10</v>
+      </c>
+      <c r="D11" t="str">
+        <f>CONCATENATE("beetle",A11,"-head")</f>
+        <v>beetle10-head</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>16</v>
+      </c>
+      <c r="G11">
+        <v>29</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11" s="4">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11" s="4">
+        <f>TabHeadParts[[#This Row],[health]]/50+TabHeadParts[[#This Row],[damage]]/25+TabHeadParts[[#This Row],[turnSpeed]]/160+TabHeadParts[[#This Row],[jumpForce]]/1300+TabHeadParts[[#This Row],[backSpeed]]/25</f>
+        <v>0.82125000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="str">
+        <f>CONCATENATE("Beetle Head ",A12)</f>
+        <v>Beetle Head 11</v>
+      </c>
+      <c r="C12" t="str">
+        <f>CONCATENATE("A ", B12)</f>
+        <v>A Beetle Head 11</v>
+      </c>
+      <c r="D12" t="str">
+        <f>CONCATENATE("beetle",A12,"-head")</f>
+        <v>beetle11-head</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>4</v>
+      </c>
+      <c r="G12">
+        <v>106</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12" s="4">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12" s="4">
+        <f>TabHeadParts[[#This Row],[health]]/50+TabHeadParts[[#This Row],[damage]]/25+TabHeadParts[[#This Row],[turnSpeed]]/160+TabHeadParts[[#This Row],[jumpForce]]/1300+TabHeadParts[[#This Row],[backSpeed]]/25</f>
+        <v>0.82250000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="str">
+        <f>CONCATENATE("Beetle Head ",A13)</f>
+        <v>Beetle Head 12</v>
+      </c>
+      <c r="C13" t="str">
+        <f>CONCATENATE("A ", B13)</f>
+        <v>A Beetle Head 12</v>
+      </c>
+      <c r="D13" t="str">
+        <f>CONCATENATE("beetle",A13,"-head")</f>
+        <v>beetle12-head</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>14</v>
+      </c>
+      <c r="G13">
+        <v>42</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13" s="4">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13" s="4">
+        <f>TabHeadParts[[#This Row],[health]]/50+TabHeadParts[[#This Row],[damage]]/25+TabHeadParts[[#This Row],[turnSpeed]]/160+TabHeadParts[[#This Row],[jumpForce]]/1300+TabHeadParts[[#This Row],[backSpeed]]/25</f>
+        <v>0.82250000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="str">
+        <f>CONCATENATE("Beetle Head ",A14)</f>
+        <v>Beetle Head 13</v>
+      </c>
+      <c r="C14" t="str">
+        <f>CONCATENATE("A ", B14)</f>
+        <v>A Beetle Head 13</v>
+      </c>
+      <c r="D14" t="str">
+        <f>CONCATENATE("beetle",A14,"-head")</f>
+        <v>beetle13-head</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>18</v>
+      </c>
+      <c r="G14">
+        <v>16</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14" s="4">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14" s="4">
+        <f>TabHeadParts[[#This Row],[health]]/50+TabHeadParts[[#This Row],[damage]]/25+TabHeadParts[[#This Row],[turnSpeed]]/160+TabHeadParts[[#This Row],[jumpForce]]/1300+TabHeadParts[[#This Row],[backSpeed]]/25</f>
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="str">
+        <f>CONCATENATE("Beetle Head ",A15)</f>
+        <v>Beetle Head 14</v>
+      </c>
+      <c r="C15" t="str">
+        <f>CONCATENATE("A ", B15)</f>
+        <v>A Beetle Head 14</v>
+      </c>
+      <c r="D15" t="str">
+        <f>CONCATENATE("beetle",A15,"-head")</f>
+        <v>beetle14-head</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>6</v>
+      </c>
+      <c r="G15">
+        <v>93</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15" s="4">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15" s="4">
+        <f>TabHeadParts[[#This Row],[health]]/50+TabHeadParts[[#This Row],[damage]]/25+TabHeadParts[[#This Row],[turnSpeed]]/160+TabHeadParts[[#This Row],[jumpForce]]/1300+TabHeadParts[[#This Row],[backSpeed]]/25</f>
+        <v>0.82125000000000004</v>
       </c>
     </row>
   </sheetData>
@@ -1138,10 +1367,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1210,10 +1439,10 @@
         <v>beetle1-thorax</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F2">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -1249,13 +1478,13 @@
         <v>beetle2-thorax</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <v>700</v>
@@ -1268,7 +1497,7 @@
       </c>
       <c r="K3">
         <f>TabThoraxParts[[#This Row],[health]]/50+TabThoraxParts[[#This Row],[damage]]/25+TabThoraxParts[[#This Row],[turnSpeed]]/160+TabThoraxParts[[#This Row],[jumpForce]]/1300+TabThoraxParts[[#This Row],[backSpeed]]/25+1/TabThoraxParts[[#This Row],[jumpCooldown]]/1.35</f>
-        <v>2.32781339031339</v>
+        <v>2.3303133903133899</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1327,13 +1556,13 @@
         <v>beetle4-thorax</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F5">
         <v>10</v>
       </c>
       <c r="G5">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="H5">
         <v>900</v>
@@ -1346,7 +1575,7 @@
       </c>
       <c r="K5">
         <f>TabThoraxParts[[#This Row],[health]]/50+TabThoraxParts[[#This Row],[damage]]/25+TabThoraxParts[[#This Row],[turnSpeed]]/160+TabThoraxParts[[#This Row],[jumpForce]]/1300+TabThoraxParts[[#This Row],[backSpeed]]/25+1/TabThoraxParts[[#This Row],[jumpCooldown]]/1.35</f>
-        <v>2.3307336182336185</v>
+        <v>2.3382336182336179</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1405,10 +1634,10 @@
         <v>beetle6-thorax</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F7">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -1483,13 +1712,13 @@
         <v>beetle8-thorax</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F9">
         <v>12</v>
       </c>
       <c r="G9">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="H9">
         <v>800</v>
@@ -1502,7 +1731,7 @@
       </c>
       <c r="K9">
         <f>TabThoraxParts[[#This Row],[health]]/50+TabThoraxParts[[#This Row],[damage]]/25+TabThoraxParts[[#This Row],[turnSpeed]]/160+TabThoraxParts[[#This Row],[jumpForce]]/1300+TabThoraxParts[[#This Row],[backSpeed]]/25+1/TabThoraxParts[[#This Row],[jumpCooldown]]/1.35</f>
-        <v>2.3098356735856735</v>
+        <v>2.3335856735856737</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1522,10 +1751,10 @@
         <v>beetle9-thorax</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="F10">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -1544,8 +1773,203 @@
         <v>2.3290028490028489</v>
       </c>
     </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="str">
+        <f>CONCATENATE("Beetle Thorax ",A11)</f>
+        <v>Beetle Thorax 10</v>
+      </c>
+      <c r="C11" t="str">
+        <f>CONCATENATE("A ", B11)</f>
+        <v>A Beetle Thorax 10</v>
+      </c>
+      <c r="D11" s="4" t="str">
+        <f>CONCATENATE("beetle",A11,"-thorax")</f>
+        <v>beetle10-thorax</v>
+      </c>
+      <c r="E11">
+        <v>21</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>1100</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0.7</v>
+      </c>
+      <c r="K11" s="4">
+        <f>TabThoraxParts[[#This Row],[health]]/50+TabThoraxParts[[#This Row],[damage]]/25+TabThoraxParts[[#This Row],[turnSpeed]]/160+TabThoraxParts[[#This Row],[jumpForce]]/1300+TabThoraxParts[[#This Row],[backSpeed]]/25+1/TabThoraxParts[[#This Row],[jumpCooldown]]/1.35</f>
+        <v>2.3243549043549043</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="str">
+        <f>CONCATENATE("Beetle Thorax ",A12)</f>
+        <v>Beetle Thorax 11</v>
+      </c>
+      <c r="C12" t="str">
+        <f>CONCATENATE("A ", B12)</f>
+        <v>A Beetle Thorax 11</v>
+      </c>
+      <c r="D12" s="4" t="str">
+        <f>CONCATENATE("beetle",A12,"-thorax")</f>
+        <v>beetle11-thorax</v>
+      </c>
+      <c r="E12">
+        <v>25</v>
+      </c>
+      <c r="F12">
+        <v>10</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>800</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0.9</v>
+      </c>
+      <c r="K12" s="4">
+        <f>TabThoraxParts[[#This Row],[health]]/50+TabThoraxParts[[#This Row],[damage]]/25+TabThoraxParts[[#This Row],[turnSpeed]]/160+TabThoraxParts[[#This Row],[jumpForce]]/1300+TabThoraxParts[[#This Row],[backSpeed]]/25+1/TabThoraxParts[[#This Row],[jumpCooldown]]/1.35</f>
+        <v>2.3384298828743271</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="str">
+        <f>CONCATENATE("Beetle Thorax ",A13)</f>
+        <v>Beetle Thorax 12</v>
+      </c>
+      <c r="C13" t="str">
+        <f>CONCATENATE("A ", B13)</f>
+        <v>A Beetle Thorax 12</v>
+      </c>
+      <c r="D13" s="4" t="str">
+        <f>CONCATENATE("beetle",A13,"-thorax")</f>
+        <v>beetle12-thorax</v>
+      </c>
+      <c r="E13">
+        <v>51</v>
+      </c>
+      <c r="F13">
+        <v>-7</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>1000</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0.9</v>
+      </c>
+      <c r="K13" s="4">
+        <f>TabThoraxParts[[#This Row],[health]]/50+TabThoraxParts[[#This Row],[damage]]/25+TabThoraxParts[[#This Row],[turnSpeed]]/160+TabThoraxParts[[#This Row],[jumpForce]]/1300+TabThoraxParts[[#This Row],[backSpeed]]/25+1/TabThoraxParts[[#This Row],[jumpCooldown]]/1.35</f>
+        <v>2.3322760367204811</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="str">
+        <f>CONCATENATE("Beetle Thorax ",A14)</f>
+        <v>Beetle Thorax 13</v>
+      </c>
+      <c r="C14" t="str">
+        <f>CONCATENATE("A ", B14)</f>
+        <v>A Beetle Thorax 13</v>
+      </c>
+      <c r="D14" s="4" t="str">
+        <f>CONCATENATE("beetle",A14,"-thorax")</f>
+        <v>beetle13-thorax</v>
+      </c>
+      <c r="E14">
+        <v>-10</v>
+      </c>
+      <c r="F14">
+        <v>10</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>1400</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0.7</v>
+      </c>
+      <c r="K14" s="4">
+        <f>TabThoraxParts[[#This Row],[health]]/50+TabThoraxParts[[#This Row],[damage]]/25+TabThoraxParts[[#This Row],[turnSpeed]]/160+TabThoraxParts[[#This Row],[jumpForce]]/1300+TabThoraxParts[[#This Row],[backSpeed]]/25+1/TabThoraxParts[[#This Row],[jumpCooldown]]/1.35</f>
+        <v>2.335124135124135</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4" t="str">
+        <f>CONCATENATE("Beetle Thorax ",A15)</f>
+        <v>Beetle Thorax 14</v>
+      </c>
+      <c r="C15" t="str">
+        <f>CONCATENATE("A ", B15)</f>
+        <v>A Beetle Thorax 14</v>
+      </c>
+      <c r="D15" s="4" t="str">
+        <f>CONCATENATE("beetle",A15,"-thorax")</f>
+        <v>beetle14-thorax</v>
+      </c>
+      <c r="E15">
+        <v>9</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>1200</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0.6</v>
+      </c>
+      <c r="K15" s="4">
+        <f>TabThoraxParts[[#This Row],[health]]/50+TabThoraxParts[[#This Row],[damage]]/25+TabThoraxParts[[#This Row],[turnSpeed]]/160+TabThoraxParts[[#This Row],[jumpForce]]/1300+TabThoraxParts[[#This Row],[backSpeed]]/25+1/TabThoraxParts[[#This Row],[jumpCooldown]]/1.35</f>
+        <v>2.3376448243114911</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="K2:K10">
+  <conditionalFormatting sqref="K2:K15">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -1566,10 +1990,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1716,10 +2140,10 @@
         <v>beetle3-abdomen</v>
       </c>
       <c r="E4">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -1728,14 +2152,14 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="J4">
         <v>0</v>
       </c>
       <c r="K4">
         <f>TabAbdomenParts[[#This Row],[health]]/50+TabAbdomenParts[[#This Row],[damage]]/25+TabAbdomenParts[[#This Row],[turnSpeed]]/160+TabAbdomenParts[[#This Row],[jumpForce]]/1300+TabAbdomenParts[[#This Row],[backSpeed]]/25</f>
-        <v>1.7</v>
+        <v>1.7000000000000002</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1755,10 +2179,10 @@
         <v>beetle4-abdomen</v>
       </c>
       <c r="E5">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -1767,14 +2191,14 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="J5">
         <v>0</v>
       </c>
       <c r="K5">
         <f>TabAbdomenParts[[#This Row],[health]]/50+TabAbdomenParts[[#This Row],[damage]]/25+TabAbdomenParts[[#This Row],[turnSpeed]]/160+TabAbdomenParts[[#This Row],[jumpForce]]/1300+TabAbdomenParts[[#This Row],[backSpeed]]/25</f>
-        <v>1.72</v>
+        <v>1.7199999999999998</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1794,10 +2218,10 @@
         <v>beetle5-abdomen</v>
       </c>
       <c r="E6">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -1806,14 +2230,14 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="J6">
         <v>0</v>
       </c>
       <c r="K6">
         <f>TabAbdomenParts[[#This Row],[health]]/50+TabAbdomenParts[[#This Row],[damage]]/25+TabAbdomenParts[[#This Row],[turnSpeed]]/160+TabAbdomenParts[[#This Row],[jumpForce]]/1300+TabAbdomenParts[[#This Row],[backSpeed]]/25</f>
-        <v>1.7</v>
+        <v>1.7000000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1833,7 +2257,7 @@
         <v>beetle6-abdomen</v>
       </c>
       <c r="E7">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -1845,14 +2269,14 @@
         <v>0</v>
       </c>
       <c r="I7">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="J7">
         <v>0</v>
       </c>
       <c r="K7">
         <f>TabAbdomenParts[[#This Row],[health]]/50+TabAbdomenParts[[#This Row],[damage]]/25+TabAbdomenParts[[#This Row],[turnSpeed]]/160+TabAbdomenParts[[#This Row],[jumpForce]]/1300+TabAbdomenParts[[#This Row],[backSpeed]]/25</f>
-        <v>1.7000000000000002</v>
+        <v>1.7200000000000002</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1911,10 +2335,10 @@
         <v>beetle8-abdomen</v>
       </c>
       <c r="E9">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -1923,14 +2347,14 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="J9">
         <v>0</v>
       </c>
       <c r="K9">
         <f>TabAbdomenParts[[#This Row],[health]]/50+TabAbdomenParts[[#This Row],[damage]]/25+TabAbdomenParts[[#This Row],[turnSpeed]]/160+TabAbdomenParts[[#This Row],[jumpForce]]/1300+TabAbdomenParts[[#This Row],[backSpeed]]/25</f>
-        <v>1.7200000000000002</v>
+        <v>1.72</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1950,10 +2374,10 @@
         <v>beetle9-abdomen</v>
       </c>
       <c r="E10">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -1962,18 +2386,213 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="J10">
         <v>0</v>
       </c>
       <c r="K10">
         <f>TabAbdomenParts[[#This Row],[health]]/50+TabAbdomenParts[[#This Row],[damage]]/25+TabAbdomenParts[[#This Row],[turnSpeed]]/160+TabAbdomenParts[[#This Row],[jumpForce]]/1300+TabAbdomenParts[[#This Row],[backSpeed]]/25</f>
+        <v>1.7200000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="str">
+        <f>CONCATENATE("Beetle Abdomen ",A11)</f>
+        <v>Beetle Abdomen 10</v>
+      </c>
+      <c r="C11" t="str">
+        <f>CONCATENATE("A ", B11)</f>
+        <v>A Beetle Abdomen 10</v>
+      </c>
+      <c r="D11" s="4" t="str">
+        <f>CONCATENATE("beetle",A11,"-abdomen")</f>
+        <v>beetle10-abdomen</v>
+      </c>
+      <c r="E11">
+        <v>68</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>9</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11" s="4">
+        <f>TabAbdomenParts[[#This Row],[health]]/50+TabAbdomenParts[[#This Row],[damage]]/25+TabAbdomenParts[[#This Row],[turnSpeed]]/160+TabAbdomenParts[[#This Row],[jumpForce]]/1300+TabAbdomenParts[[#This Row],[backSpeed]]/25</f>
+        <v>1.7200000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="str">
+        <f>CONCATENATE("Beetle Abdomen ",A12)</f>
+        <v>Beetle Abdomen 11</v>
+      </c>
+      <c r="C12" t="str">
+        <f>CONCATENATE("A ", B12)</f>
+        <v>A Beetle Abdomen 11</v>
+      </c>
+      <c r="D12" s="4" t="str">
+        <f>CONCATENATE("beetle",A12,"-abdomen")</f>
+        <v>beetle11-abdomen</v>
+      </c>
+      <c r="E12">
+        <v>74</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>6</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12" s="4">
+        <f>TabAbdomenParts[[#This Row],[health]]/50+TabAbdomenParts[[#This Row],[damage]]/25+TabAbdomenParts[[#This Row],[turnSpeed]]/160+TabAbdomenParts[[#This Row],[jumpForce]]/1300+TabAbdomenParts[[#This Row],[backSpeed]]/25</f>
         <v>1.72</v>
       </c>
     </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="str">
+        <f>CONCATENATE("Beetle Abdomen ",A13)</f>
+        <v>Beetle Abdomen 12</v>
+      </c>
+      <c r="C13" t="str">
+        <f>CONCATENATE("A ", B13)</f>
+        <v>A Beetle Abdomen 12</v>
+      </c>
+      <c r="D13" s="4" t="str">
+        <f>CONCATENATE("beetle",A13,"-abdomen")</f>
+        <v>beetle12-abdomen</v>
+      </c>
+      <c r="E13">
+        <v>65</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>8</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13" s="4">
+        <f>TabAbdomenParts[[#This Row],[health]]/50+TabAbdomenParts[[#This Row],[damage]]/25+TabAbdomenParts[[#This Row],[turnSpeed]]/160+TabAbdomenParts[[#This Row],[jumpForce]]/1300+TabAbdomenParts[[#This Row],[backSpeed]]/25</f>
+        <v>1.7000000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="str">
+        <f>CONCATENATE("Beetle Abdomen ",A14)</f>
+        <v>Beetle Abdomen 13</v>
+      </c>
+      <c r="C14" t="str">
+        <f>CONCATENATE("A ", B14)</f>
+        <v>A Beetle Abdomen 13</v>
+      </c>
+      <c r="D14" s="4" t="str">
+        <f>CONCATENATE("beetle",A14,"-abdomen")</f>
+        <v>beetle13-abdomen</v>
+      </c>
+      <c r="E14">
+        <v>63</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>11</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14" s="4">
+        <f>TabAbdomenParts[[#This Row],[health]]/50+TabAbdomenParts[[#This Row],[damage]]/25+TabAbdomenParts[[#This Row],[turnSpeed]]/160+TabAbdomenParts[[#This Row],[jumpForce]]/1300+TabAbdomenParts[[#This Row],[backSpeed]]/25</f>
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4" t="str">
+        <f>CONCATENATE("Beetle Abdomen ",A15)</f>
+        <v>Beetle Abdomen 14</v>
+      </c>
+      <c r="C15" t="str">
+        <f>CONCATENATE("A ", B15)</f>
+        <v>A Beetle Abdomen 14</v>
+      </c>
+      <c r="D15" s="4" t="str">
+        <f>CONCATENATE("beetle",A15,"-abdomen")</f>
+        <v>beetle14-abdomen</v>
+      </c>
+      <c r="E15">
+        <v>54</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>14</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15" s="4">
+        <f>TabAbdomenParts[[#This Row],[health]]/50+TabAbdomenParts[[#This Row],[damage]]/25+TabAbdomenParts[[#This Row],[turnSpeed]]/160+TabAbdomenParts[[#This Row],[jumpForce]]/1300+TabAbdomenParts[[#This Row],[backSpeed]]/25</f>
+        <v>1.7200000000000002</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="K2:K10">
+  <conditionalFormatting sqref="K2:K15">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -1997,8 +2616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2079,14 +2698,14 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="J2">
         <v>0</v>
       </c>
       <c r="K2" s="2">
         <f>TabLegParts[[#This Row],[health]]/50+TabLegParts[[#This Row],[damage]]/25+TabLegParts[[#This Row],[turnSpeed]]/160+TabLegParts[[#This Row],[jumpForce]]/1300+TabLegParts[[#This Row],[backSpeed]]/25</f>
-        <v>0.995</v>
+        <v>0.755</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -2112,20 +2731,20 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="J3">
         <v>0</v>
       </c>
       <c r="K3" s="3">
         <f>TabLegParts[[#This Row],[health]]/50+TabLegParts[[#This Row],[damage]]/25+TabLegParts[[#This Row],[turnSpeed]]/160+TabLegParts[[#This Row],[jumpForce]]/1300+TabLegParts[[#This Row],[backSpeed]]/25</f>
-        <v>0.97499999999999998</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -2151,20 +2770,20 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="J4">
         <v>0</v>
       </c>
       <c r="K4" s="2">
         <f>TabLegParts[[#This Row],[health]]/50+TabLegParts[[#This Row],[damage]]/25+TabLegParts[[#This Row],[turnSpeed]]/160+TabLegParts[[#This Row],[jumpForce]]/1300+TabLegParts[[#This Row],[backSpeed]]/25</f>
-        <v>0.98499999999999999</v>
+        <v>0.75124999999999997</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -2196,14 +2815,14 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J5">
         <v>0</v>
       </c>
       <c r="K5" s="3">
         <f>TabLegParts[[#This Row],[health]]/50+TabLegParts[[#This Row],[damage]]/25+TabLegParts[[#This Row],[turnSpeed]]/160+TabLegParts[[#This Row],[jumpForce]]/1300+TabLegParts[[#This Row],[backSpeed]]/25</f>
-        <v>0.99</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -2229,20 +2848,20 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>40</v>
+        <v>82</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="J6">
         <v>0</v>
       </c>
       <c r="K6" s="2">
         <f>TabLegParts[[#This Row],[health]]/50+TabLegParts[[#This Row],[damage]]/25+TabLegParts[[#This Row],[turnSpeed]]/160+TabLegParts[[#This Row],[jumpForce]]/1300+TabLegParts[[#This Row],[backSpeed]]/25</f>
-        <v>0.97</v>
+        <v>0.75249999999999995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>